<commit_message>
commit from 14.03.24 - changing in replying messages and trying ssh
</commit_message>
<xml_diff>
--- a/lists/IP echipamente statii.xlsx
+++ b/lists/IP echipamente statii.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\node whatsap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\TPL_Alerts2.0\lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3621041-9C48-43A1-A44E-6C859B277742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A156D0B-7AA9-4F8A-A91E-F234DF566C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1872" yWindow="1872" windowWidth="17280" windowHeight="9108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista principala" sheetId="1" r:id="rId1"/>
@@ -1030,10 +1030,10 @@
     <t>Releu Panou</t>
   </si>
   <si>
-    <t>192.168.95.72</t>
-  </si>
-  <si>
     <t>192.168.95.71</t>
+  </si>
+  <si>
+    <t>192.168.35.52</t>
   </si>
 </sst>
 </file>
@@ -2011,7 +2011,7 @@
   <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2088,10 +2088,10 @@
         <v>177</v>
       </c>
       <c r="G2" s="17" t="s">
+        <v>335</v>
+      </c>
+      <c r="H2" s="17" t="s">
         <v>336</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>335</v>
       </c>
       <c r="I2" s="34"/>
       <c r="J2" s="30"/>

</xml_diff>

<commit_message>
a version from 25.03.24. Note that LocalAuth is not working correctly, you should scan QR every time start app.
</commit_message>
<xml_diff>
--- a/lists/IP echipamente statii.xlsx
+++ b/lists/IP echipamente statii.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\TPL_Alerts2.0\lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A156D0B-7AA9-4F8A-A91E-F234DF566C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD639C4-E7E3-4F2E-9B81-AA4DD923FD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1872" yWindow="1872" windowWidth="17280" windowHeight="9108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista principala" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="335">
   <si>
     <t>Buffer maro</t>
   </si>
@@ -1028,12 +1028,6 @@
   </si>
   <si>
     <t>Releu Panou</t>
-  </si>
-  <si>
-    <t>192.168.95.71</t>
-  </si>
-  <si>
-    <t>192.168.35.52</t>
   </si>
 </sst>
 </file>
@@ -2011,7 +2005,7 @@
   <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2087,12 +2081,8 @@
       <c r="F2" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="G2" s="17" t="s">
-        <v>335</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>336</v>
-      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
       <c r="I2" s="34"/>
       <c r="J2" s="30"/>
       <c r="K2" s="31" t="s">

</xml_diff>

<commit_message>
Issue with whatsapp-web start is temporarely solved by using local Auth with sessions
</commit_message>
<xml_diff>
--- a/lists/IP echipamente statii.xlsx
+++ b/lists/IP echipamente statii.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\TPL_Alerts2.0\lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD639C4-E7E3-4F2E-9B81-AA4DD923FD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC459951-A6A6-4650-AB32-78D2BB321BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="337">
   <si>
     <t>Buffer maro</t>
   </si>
@@ -1028,6 +1028,12 @@
   </si>
   <si>
     <t>Releu Panou</t>
+  </si>
+  <si>
+    <t>192.168.35.53</t>
+  </si>
+  <si>
+    <t>192.168.35.52</t>
   </si>
 </sst>
 </file>
@@ -2004,8 +2010,8 @@
   </sheetPr>
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3595,8 +3601,12 @@
       <c r="F58" s="17" t="s">
         <v>298</v>
       </c>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
+      <c r="G58" s="17" t="s">
+        <v>335</v>
+      </c>
+      <c r="H58" s="17" t="s">
+        <v>336</v>
+      </c>
       <c r="I58" s="34"/>
       <c r="J58" s="30"/>
       <c r="K58" s="11"/>

</xml_diff>

<commit_message>
solve new whatsapp lib issue
</commit_message>
<xml_diff>
--- a/lists/IP echipamente statii.xlsx
+++ b/lists/IP echipamente statii.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\TPL_Alerts2.0\lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC459951-A6A6-4650-AB32-78D2BB321BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9075D26C-6D4C-4326-B83F-090E94AF7386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista principala" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="338">
   <si>
     <t>Buffer maro</t>
   </si>
@@ -574,466 +574,469 @@
     <t>clasa 35 - de la 81</t>
   </si>
   <si>
+    <t>192.168.35.31</t>
+  </si>
+  <si>
+    <t>192.168.35.76 (spre IRIC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clasa 45 - de la 64 + 77 si 78 </t>
+  </si>
+  <si>
+    <t>192.168.25.21</t>
+  </si>
+  <si>
+    <t>192.168.95.141</t>
+  </si>
+  <si>
+    <t>192.168.25.23</t>
+  </si>
+  <si>
+    <t>192.168.25.55</t>
+  </si>
+  <si>
+    <t>clasa 55  - de la 52</t>
+  </si>
+  <si>
+    <t>192.168.25.25</t>
+  </si>
+  <si>
+    <t>192.168.25.26</t>
+  </si>
+  <si>
+    <t>192.168.25.28</t>
+  </si>
+  <si>
+    <t>192.168.25.32</t>
+  </si>
+  <si>
+    <t>192.168.25.33(liber)</t>
+  </si>
+  <si>
+    <t>Banca spre bdj</t>
+  </si>
+  <si>
+    <t>192.168.25.41</t>
+  </si>
+  <si>
+    <t>192.168.25.42</t>
+  </si>
+  <si>
+    <t>192.168.25.43</t>
+  </si>
+  <si>
+    <t>192.168.15.21</t>
+  </si>
+  <si>
+    <t>192.168.15.22</t>
+  </si>
+  <si>
+    <t>192.168.55.21</t>
+  </si>
+  <si>
+    <t>192.168.95.149</t>
+  </si>
+  <si>
+    <t>192.168.55.26</t>
+  </si>
+  <si>
+    <t>192.168.55.47 statie 192.168.55.50 cctv lidl</t>
+  </si>
+  <si>
+    <t>53 si 54 adaugate fata de lista originala 08.10.2021</t>
+  </si>
+  <si>
+    <t>192.168.55.28</t>
+  </si>
+  <si>
+    <t>192.168.95.148</t>
+  </si>
+  <si>
+    <t>192.168.55.30</t>
+  </si>
+  <si>
+    <t>192.168.55.38</t>
+  </si>
+  <si>
+    <t>192.168.95.146</t>
+  </si>
+  <si>
+    <t>192.168.55.40</t>
+  </si>
+  <si>
+    <t>192.168.55.51 statie</t>
+  </si>
+  <si>
+    <t>192.168.45.21</t>
+  </si>
+  <si>
+    <t>192.168.45.53 (CCTV)  192.168.45.54 (statie)</t>
+  </si>
+  <si>
+    <t>192.168.45.23</t>
+  </si>
+  <si>
+    <t>192.168.45.24</t>
+  </si>
+  <si>
+    <t>192.168.45.59 statie</t>
+  </si>
+  <si>
+    <t>192.168.45.58 cctv</t>
+  </si>
+  <si>
+    <t>192.168.15.24</t>
+  </si>
+  <si>
+    <t>192.168.15.25</t>
+  </si>
+  <si>
+    <t>Banca spre primarie</t>
+  </si>
+  <si>
+    <t>192.168.25.46</t>
+  </si>
+  <si>
+    <t>cctv 192.168.2.66 eth disabled</t>
+  </si>
+  <si>
+    <t>192.168.25.35</t>
+  </si>
+  <si>
+    <t>192.168.25.36</t>
+  </si>
+  <si>
+    <t>192.168.25.30</t>
+  </si>
+  <si>
+    <t>192.168.25.50</t>
+  </si>
+  <si>
+    <t>192.168.25.48</t>
+  </si>
+  <si>
+    <t>192.168.25.59 statie   192.168.25.60 cctv</t>
+  </si>
+  <si>
+    <t>192.168.25.51</t>
+  </si>
+  <si>
+    <t>192.168.25.56</t>
+  </si>
+  <si>
+    <t>192.168.95.143</t>
+  </si>
+  <si>
+    <t>192.168.35.34</t>
+  </si>
+  <si>
+    <t>192.168.35.35</t>
+  </si>
+  <si>
+    <t>192.168.35.37</t>
+  </si>
+  <si>
+    <t>192.168.35.38</t>
+  </si>
+  <si>
+    <t>192.168.35.40</t>
+  </si>
+  <si>
+    <t>192.168.35.41</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 192.168.35.42             192.168.35.43    CCTV</t>
+  </si>
+  <si>
+    <t>192.168.55.34</t>
+  </si>
+  <si>
+    <t>192.168.55.36</t>
+  </si>
+  <si>
+    <t>192.168.55.46 cctv 192.168.55.52 statie de configurat</t>
+  </si>
+  <si>
+    <t>192.168.35.45</t>
+  </si>
+  <si>
+    <t>192.168.35.46</t>
+  </si>
+  <si>
+    <t>192.168.35.48</t>
+  </si>
+  <si>
+    <t>192.168.35.49</t>
+  </si>
+  <si>
+    <t>192.168.35.74 192.168.35.75 cctv</t>
+  </si>
+  <si>
+    <t>192.168.45.26</t>
+  </si>
+  <si>
+    <t>192.168.45.55 statie 192.168.45.58 cctv</t>
+  </si>
+  <si>
+    <t>55 adaugat fata de lista originala 8.10.2021</t>
+  </si>
+  <si>
+    <t>192.168.55.42</t>
+  </si>
+  <si>
+    <t>192.168.55.48 statie ap 192.168.55.49 cctv</t>
+  </si>
+  <si>
+    <t>192.168.55.44</t>
+  </si>
+  <si>
+    <t>192.168.55.45</t>
+  </si>
+  <si>
+    <t>192.168.55.22 cctv  192.168.55.23  statie</t>
+  </si>
+  <si>
+    <t>192.168.45.28</t>
+  </si>
+  <si>
+    <t>192.168.45.31</t>
+  </si>
+  <si>
+    <t>192.168.45.61 statie 192.168.45.62 cctv</t>
+  </si>
+  <si>
+    <t>192.168.45.50</t>
+  </si>
+  <si>
+    <t>192.168.45.49 statie                192.168.45.63</t>
+  </si>
+  <si>
+    <t>192.168.25.38</t>
+  </si>
+  <si>
+    <t>192.168.25.39 statie 192.168.25.58 cctv</t>
+  </si>
+  <si>
+    <t>192.168.95.145</t>
+  </si>
+  <si>
+    <t>192.168.35.56</t>
+  </si>
+  <si>
+    <t>192.168.35.72 192.168.35.73 cctv</t>
+  </si>
+  <si>
+    <t>pe antena de la stalpul de vizavi.Montat cutie pe stalp Sw cu fibra spre Spac</t>
+  </si>
+  <si>
+    <t>192.168.45.33</t>
+  </si>
+  <si>
+    <t>192.168.45.34</t>
+  </si>
+  <si>
+    <t>192.168.45.57 (CCTV) 192.168.45.60 statie</t>
+  </si>
+  <si>
+    <t>192.168.45.77(statie) 192.168.45.78 (cctv)</t>
+  </si>
+  <si>
+    <t>192.168.35.60</t>
+  </si>
+  <si>
+    <t>192.168.95.142</t>
+  </si>
+  <si>
+    <t>192.168.35.62</t>
+  </si>
+  <si>
+    <t>192.168.35.64</t>
+  </si>
+  <si>
+    <t>192.168.35.65</t>
+  </si>
+  <si>
+    <t>192.168.35.67</t>
+  </si>
+  <si>
+    <t>192.168.35.68</t>
+  </si>
+  <si>
+    <t>antena spre Lev tolstoi</t>
+  </si>
+  <si>
+    <t>fibra de la scoala</t>
+  </si>
+  <si>
+    <t>192.168.45.39</t>
+  </si>
+  <si>
+    <t>192.168.45.40  statie                   192.168.45.41 cctv</t>
+  </si>
+  <si>
+    <t>192.168.95.152</t>
+  </si>
+  <si>
+    <t>Aleea Dumbravii gostat</t>
+  </si>
+  <si>
+    <t>192.168.95.161</t>
+  </si>
+  <si>
+    <t>192.168.95.153</t>
+  </si>
+  <si>
+    <t>192.168.95.144</t>
+  </si>
+  <si>
+    <t>192.168.35.51</t>
+  </si>
+  <si>
+    <t>192.168.15.27</t>
+  </si>
+  <si>
+    <t>192.168.15.28</t>
+  </si>
+  <si>
+    <t>192.168.15.29 statie 192.168.15.30 cctv</t>
+  </si>
+  <si>
+    <t>192.168.35.70</t>
+  </si>
+  <si>
+    <t>192.168.95.147</t>
+  </si>
+  <si>
+    <t>192.168.35.71</t>
+  </si>
+  <si>
+    <t>A1   15.10</t>
+  </si>
+  <si>
+    <t>A2   25.11</t>
+  </si>
+  <si>
+    <t>A3   35.12</t>
+  </si>
+  <si>
+    <t>15 si 38 vin in acelasi dulap de comunicatie colt enescu - universitatii</t>
+  </si>
+  <si>
+    <t>B    45.13</t>
+  </si>
+  <si>
+    <t>C    55.3</t>
+  </si>
+  <si>
+    <t>Universitate</t>
+  </si>
+  <si>
+    <t>Centrofarm 2</t>
+  </si>
+  <si>
+    <t>Carrefour spre centru</t>
+  </si>
+  <si>
+    <t>Carrefour spre BDJ</t>
+  </si>
+  <si>
+    <t>Sticla</t>
+  </si>
+  <si>
+    <t>x192.168.35.30</t>
+  </si>
+  <si>
+    <t>192.168.45.240</t>
+  </si>
+  <si>
+    <t>Obcini Flori</t>
+  </si>
+  <si>
+    <t>Orizont spre Centru</t>
+  </si>
+  <si>
+    <t>Orizont spre BDJ</t>
+  </si>
+  <si>
+    <t>Curcubeu spre catedrala</t>
+  </si>
+  <si>
+    <t>Policlinca spre BDJ</t>
+  </si>
+  <si>
+    <t>Grup scolar spre BDJ</t>
+  </si>
+  <si>
+    <t>Centru spre primarie</t>
+  </si>
+  <si>
+    <t>Grup scolar spre centru</t>
+  </si>
+  <si>
+    <t>Mobila spre curcubeu</t>
+  </si>
+  <si>
+    <t>Bazar 2 Lidl</t>
+  </si>
+  <si>
+    <t>Bazar 1</t>
+  </si>
+  <si>
+    <t>Mobila spre obcini</t>
+  </si>
+  <si>
+    <t>Catedrala spre policlinica</t>
+  </si>
+  <si>
+    <t>192.168.35.58</t>
+  </si>
+  <si>
+    <t>Curcubeu spre obcini</t>
+  </si>
+  <si>
+    <t>x192.168.45.48</t>
+  </si>
+  <si>
+    <t>pe 49 eth disabled ,pe fibra de la statia de vizavi</t>
+  </si>
+  <si>
+    <t>x192.168.25.37</t>
+  </si>
+  <si>
+    <t>x192.168.35.63</t>
+  </si>
+  <si>
+    <t>x192.168.25.45</t>
+  </si>
+  <si>
+    <t>Autogara</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>Releu Panou</t>
+  </si>
+  <si>
+    <t>192.168.35.53</t>
+  </si>
+  <si>
+    <t>192.168.35.52</t>
+  </si>
+  <si>
     <t>192.168.95.150</t>
   </si>
   <si>
-    <t>192.168.35.31</t>
-  </si>
-  <si>
-    <t>192.168.35.76 (spre IRIC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clasa 45 - de la 64 + 77 si 78 </t>
-  </si>
-  <si>
-    <t>192.168.25.21</t>
-  </si>
-  <si>
-    <t>192.168.95.141</t>
-  </si>
-  <si>
-    <t>192.168.25.23</t>
-  </si>
-  <si>
-    <t>192.168.25.55</t>
-  </si>
-  <si>
-    <t>clasa 55  - de la 52</t>
-  </si>
-  <si>
-    <t>192.168.25.25</t>
-  </si>
-  <si>
-    <t>192.168.25.26</t>
-  </si>
-  <si>
-    <t>192.168.25.28</t>
-  </si>
-  <si>
-    <t>192.168.25.32</t>
-  </si>
-  <si>
-    <t>192.168.25.33(liber)</t>
-  </si>
-  <si>
-    <t>Banca spre bdj</t>
-  </si>
-  <si>
-    <t>192.168.25.41</t>
-  </si>
-  <si>
-    <t>192.168.25.42</t>
-  </si>
-  <si>
-    <t>192.168.25.43</t>
-  </si>
-  <si>
-    <t>192.168.15.21</t>
-  </si>
-  <si>
-    <t>192.168.15.22</t>
-  </si>
-  <si>
-    <t>192.168.55.21</t>
-  </si>
-  <si>
-    <t>192.168.95.149</t>
-  </si>
-  <si>
-    <t>192.168.55.26</t>
-  </si>
-  <si>
-    <t>192.168.55.47 statie 192.168.55.50 cctv lidl</t>
-  </si>
-  <si>
-    <t>53 si 54 adaugate fata de lista originala 08.10.2021</t>
-  </si>
-  <si>
-    <t>192.168.55.28</t>
-  </si>
-  <si>
-    <t>192.168.95.148</t>
-  </si>
-  <si>
-    <t>192.168.55.30</t>
-  </si>
-  <si>
-    <t>192.168.55.38</t>
-  </si>
-  <si>
-    <t>192.168.95.146</t>
-  </si>
-  <si>
-    <t>192.168.55.40</t>
-  </si>
-  <si>
-    <t>192.168.55.51 statie</t>
-  </si>
-  <si>
-    <t>192.168.45.21</t>
-  </si>
-  <si>
-    <t>192.168.45.53 (CCTV)  192.168.45.54 (statie)</t>
-  </si>
-  <si>
-    <t>192.168.45.23</t>
-  </si>
-  <si>
-    <t>192.168.45.24</t>
-  </si>
-  <si>
-    <t>192.168.45.59 statie</t>
-  </si>
-  <si>
-    <t>192.168.45.58 cctv</t>
-  </si>
-  <si>
-    <t>192.168.15.24</t>
-  </si>
-  <si>
-    <t>192.168.15.25</t>
-  </si>
-  <si>
-    <t>Banca spre primarie</t>
-  </si>
-  <si>
-    <t>192.168.25.46</t>
-  </si>
-  <si>
-    <t>cctv 192.168.2.66 eth disabled</t>
-  </si>
-  <si>
-    <t>192.168.25.35</t>
-  </si>
-  <si>
-    <t>192.168.25.36</t>
-  </si>
-  <si>
-    <t>192.168.25.30</t>
-  </si>
-  <si>
-    <t>192.168.25.50</t>
-  </si>
-  <si>
-    <t>192.168.25.48</t>
-  </si>
-  <si>
-    <t>192.168.25.59 statie   192.168.25.60 cctv</t>
-  </si>
-  <si>
-    <t>192.168.25.51</t>
-  </si>
-  <si>
-    <t>192.168.25.56</t>
-  </si>
-  <si>
-    <t>192.168.95.143</t>
-  </si>
-  <si>
-    <t>192.168.35.34</t>
-  </si>
-  <si>
-    <t>192.168.35.35</t>
-  </si>
-  <si>
-    <t>192.168.35.37</t>
-  </si>
-  <si>
-    <t>192.168.35.38</t>
-  </si>
-  <si>
-    <t>192.168.35.40</t>
-  </si>
-  <si>
-    <t>192.168.35.41</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 192.168.35.42             192.168.35.43    CCTV</t>
-  </si>
-  <si>
-    <t>192.168.55.34</t>
-  </si>
-  <si>
-    <t>192.168.55.36</t>
-  </si>
-  <si>
-    <t>192.168.55.46 cctv 192.168.55.52 statie de configurat</t>
-  </si>
-  <si>
-    <t>192.168.35.45</t>
-  </si>
-  <si>
-    <t>192.168.35.46</t>
-  </si>
-  <si>
-    <t>192.168.35.48</t>
-  </si>
-  <si>
-    <t>192.168.35.49</t>
-  </si>
-  <si>
-    <t>192.168.35.74 192.168.35.75 cctv</t>
-  </si>
-  <si>
-    <t>192.168.45.26</t>
-  </si>
-  <si>
-    <t>192.168.45.55 statie 192.168.45.58 cctv</t>
-  </si>
-  <si>
-    <t>55 adaugat fata de lista originala 8.10.2021</t>
-  </si>
-  <si>
-    <t>192.168.55.42</t>
-  </si>
-  <si>
-    <t>192.168.55.48 statie ap 192.168.55.49 cctv</t>
-  </si>
-  <si>
-    <t>192.168.55.32</t>
-  </si>
-  <si>
-    <t>192.168.55.44</t>
-  </si>
-  <si>
-    <t>192.168.55.45</t>
-  </si>
-  <si>
-    <t>192.168.55.22 cctv  192.168.55.23  statie</t>
-  </si>
-  <si>
-    <t>192.168.45.28</t>
-  </si>
-  <si>
-    <t>192.168.45.31</t>
-  </si>
-  <si>
-    <t>192.168.45.61 statie 192.168.45.62 cctv</t>
-  </si>
-  <si>
-    <t>192.168.45.50</t>
-  </si>
-  <si>
-    <t>192.168.45.49 statie                192.168.45.63</t>
-  </si>
-  <si>
-    <t>192.168.25.38</t>
-  </si>
-  <si>
-    <t>192.168.25.39 statie 192.168.25.58 cctv</t>
-  </si>
-  <si>
-    <t>192.168.95.145</t>
-  </si>
-  <si>
-    <t>192.168.35.56</t>
-  </si>
-  <si>
-    <t>192.168.35.72 192.168.35.73 cctv</t>
-  </si>
-  <si>
-    <t>pe antena de la stalpul de vizavi.Montat cutie pe stalp Sw cu fibra spre Spac</t>
-  </si>
-  <si>
-    <t>192.168.45.33</t>
-  </si>
-  <si>
-    <t>192.168.45.34</t>
-  </si>
-  <si>
-    <t>192.168.45.57 (CCTV) 192.168.45.60 statie</t>
+    <t>x192.168.95.160</t>
   </si>
   <si>
     <t>192.168.45.45</t>
   </si>
   <si>
-    <t>192.168.45.77(statie) 192.168.45.78 (cctv)</t>
-  </si>
-  <si>
-    <t>192.168.35.60</t>
-  </si>
-  <si>
-    <t>192.168.95.142</t>
-  </si>
-  <si>
-    <t>192.168.35.62</t>
-  </si>
-  <si>
-    <t>192.168.35.64</t>
-  </si>
-  <si>
-    <t>192.168.35.65</t>
-  </si>
-  <si>
-    <t>192.168.35.67</t>
-  </si>
-  <si>
-    <t>192.168.35.68</t>
-  </si>
-  <si>
-    <t>antena spre Lev tolstoi</t>
-  </si>
-  <si>
-    <t>fibra de la scoala</t>
-  </si>
-  <si>
-    <t>192.168.45.39</t>
-  </si>
-  <si>
-    <t>192.168.45.40  statie                   192.168.45.41 cctv</t>
-  </si>
-  <si>
-    <t>192.168.95.160</t>
-  </si>
-  <si>
-    <t>192.168.95.152</t>
-  </si>
-  <si>
-    <t>Aleea Dumbravii gostat</t>
-  </si>
-  <si>
-    <t>192.168.95.161</t>
-  </si>
-  <si>
-    <t>192.168.95.153</t>
-  </si>
-  <si>
-    <t>192.168.95.144</t>
-  </si>
-  <si>
-    <t>192.168.35.51</t>
-  </si>
-  <si>
-    <t>192.168.15.27</t>
-  </si>
-  <si>
-    <t>192.168.15.28</t>
-  </si>
-  <si>
-    <t>192.168.15.29 statie 192.168.15.30 cctv</t>
-  </si>
-  <si>
-    <t>192.168.35.70</t>
-  </si>
-  <si>
-    <t>192.168.95.147</t>
-  </si>
-  <si>
-    <t>192.168.35.71</t>
-  </si>
-  <si>
-    <t>A1   15.10</t>
-  </si>
-  <si>
-    <t>A2   25.11</t>
-  </si>
-  <si>
-    <t>A3   35.12</t>
-  </si>
-  <si>
-    <t>15 si 38 vin in acelasi dulap de comunicatie colt enescu - universitatii</t>
-  </si>
-  <si>
-    <t>B    45.13</t>
-  </si>
-  <si>
-    <t>C    55.3</t>
-  </si>
-  <si>
-    <t>Universitate</t>
-  </si>
-  <si>
-    <t>Centrofarm 2</t>
-  </si>
-  <si>
-    <t>Carrefour spre centru</t>
-  </si>
-  <si>
-    <t>Carrefour spre BDJ</t>
-  </si>
-  <si>
-    <t>Sticla</t>
-  </si>
-  <si>
-    <t>x192.168.35.30</t>
-  </si>
-  <si>
-    <t>192.168.45.240</t>
-  </si>
-  <si>
-    <t>Obcini Flori</t>
-  </si>
-  <si>
-    <t>Orizont spre Centru</t>
-  </si>
-  <si>
-    <t>Orizont spre BDJ</t>
-  </si>
-  <si>
-    <t>Curcubeu spre catedrala</t>
-  </si>
-  <si>
-    <t>Policlinca spre BDJ</t>
-  </si>
-  <si>
-    <t>Grup scolar spre BDJ</t>
-  </si>
-  <si>
-    <t>Centru spre primarie</t>
-  </si>
-  <si>
-    <t>Grup scolar spre centru</t>
-  </si>
-  <si>
-    <t>Mobila spre curcubeu</t>
-  </si>
-  <si>
-    <t>Bazar 2 Lidl</t>
-  </si>
-  <si>
-    <t>Bazar 1</t>
-  </si>
-  <si>
-    <t>Mobila spre obcini</t>
-  </si>
-  <si>
-    <t>Catedrala spre policlinica</t>
-  </si>
-  <si>
-    <t>192.168.35.58</t>
-  </si>
-  <si>
-    <t>Curcubeu spre obcini</t>
-  </si>
-  <si>
-    <t>x192.168.45.48</t>
-  </si>
-  <si>
-    <t>pe 49 eth disabled ,pe fibra de la statia de vizavi</t>
-  </si>
-  <si>
-    <t>x192.168.25.37</t>
-  </si>
-  <si>
-    <t>x192.168.35.63</t>
-  </si>
-  <si>
-    <t>x192.168.25.45</t>
-  </si>
-  <si>
-    <t>Autogara</t>
-  </si>
-  <si>
-    <t>AP</t>
-  </si>
-  <si>
-    <t>Releu Panou</t>
-  </si>
-  <si>
-    <t>192.168.35.53</t>
-  </si>
-  <si>
-    <t>192.168.35.52</t>
+    <t>x192.168.55.32</t>
+  </si>
+  <si>
+    <t>x192.168.55.31</t>
   </si>
 </sst>
 </file>
@@ -2010,28 +2013,28 @@
   </sheetPr>
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="63" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="19.42578125" style="63" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" style="63" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19.44140625" style="63" customWidth="1"/>
+    <col min="9" max="9" width="21.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>171</v>
       </c>
@@ -2051,10 +2054,10 @@
         <v>50</v>
       </c>
       <c r="G1" s="75" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="H1" s="75" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="I1" s="29" t="s">
         <v>47</v>
@@ -2068,7 +2071,7 @@
       <c r="N1" s="33"/>
       <c r="O1" s="33"/>
     </row>
-    <row r="2" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -2099,12 +2102,12 @@
       <c r="N2" s="33"/>
       <c r="O2" s="33"/>
     </row>
-    <row r="3" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>60</v>
@@ -2130,88 +2133,88 @@
       <c r="N3" s="33"/>
       <c r="O3" s="33"/>
     </row>
-    <row r="4" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="66" t="s">
         <v>62</v>
       </c>
       <c r="D4" s="20"/>
-      <c r="E4" s="17" t="s">
-        <v>183</v>
+      <c r="E4" s="66" t="s">
+        <v>333</v>
       </c>
       <c r="F4" s="65" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
       <c r="I4" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="J4" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="J4" s="30" t="s">
+      <c r="K4" s="31" t="s">
         <v>185</v>
-      </c>
-      <c r="K4" s="31" t="s">
-        <v>186</v>
       </c>
       <c r="L4" s="31"/>
       <c r="M4" s="31"/>
       <c r="N4" s="33"/>
       <c r="O4" s="33"/>
     </row>
-    <row r="5" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>64</v>
       </c>
       <c r="D5" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="F5" s="17" t="s">
         <v>188</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>189</v>
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="17"/>
       <c r="I5" s="34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J5" s="30"/>
       <c r="K5" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L5" s="31"/>
       <c r="M5" s="31"/>
       <c r="N5" s="33"/>
       <c r="O5" s="33"/>
     </row>
-    <row r="6" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>5</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>66</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E6" s="35"/>
       <c r="F6" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
@@ -2223,7 +2226,7 @@
       <c r="N6" s="33"/>
       <c r="O6" s="33"/>
     </row>
-    <row r="7" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>6</v>
       </c>
@@ -2244,12 +2247,12 @@
       <c r="N7" s="33"/>
       <c r="O7" s="33"/>
     </row>
-    <row r="8" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>7</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>69</v>
@@ -2257,7 +2260,7 @@
       <c r="D8" s="20"/>
       <c r="E8" s="35"/>
       <c r="F8" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
@@ -2269,12 +2272,12 @@
       <c r="N8" s="31"/>
       <c r="O8" s="33"/>
     </row>
-    <row r="9" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>72</v>
@@ -2282,12 +2285,12 @@
       <c r="D9" s="20"/>
       <c r="E9" s="35"/>
       <c r="F9" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
       <c r="I9" s="36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J9" s="30"/>
       <c r="K9" s="30"/>
@@ -2296,27 +2299,27 @@
       <c r="N9" s="31"/>
       <c r="O9" s="33"/>
     </row>
-    <row r="10" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16">
         <v>9</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>95</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E10" s="35"/>
       <c r="F10" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
       <c r="I10" s="36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J10" s="30"/>
       <c r="K10" s="30"/>
@@ -2325,7 +2328,7 @@
       <c r="N10" s="31"/>
       <c r="O10" s="33"/>
     </row>
-    <row r="11" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16">
         <v>10</v>
       </c>
@@ -2336,11 +2339,11 @@
         <v>77</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E11" s="35"/>
       <c r="F11" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
@@ -2352,7 +2355,7 @@
       <c r="N11" s="31"/>
       <c r="O11" s="33"/>
     </row>
-    <row r="12" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16">
         <v>11</v>
       </c>
@@ -2365,7 +2368,7 @@
       <c r="D12" s="20"/>
       <c r="E12" s="35"/>
       <c r="F12" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
@@ -2377,55 +2380,55 @@
       <c r="N12" s="31"/>
       <c r="O12" s="33"/>
     </row>
-    <row r="13" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16">
         <v>12</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>81</v>
       </c>
       <c r="D13" s="20"/>
-      <c r="E13" s="35" t="s">
+      <c r="E13" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="F13" s="17" t="s">
         <v>204</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>205</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
       <c r="I13" s="34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J13" s="11"/>
       <c r="K13" s="40" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L13" s="31"/>
       <c r="M13" s="31"/>
       <c r="N13" s="31"/>
       <c r="O13" s="33"/>
     </row>
-    <row r="14" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
         <v>13</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>83</v>
       </c>
       <c r="D14" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="F14" s="17" t="s">
         <v>209</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>210</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -2437,29 +2440,29 @@
       <c r="N14" s="33"/>
       <c r="O14" s="33"/>
     </row>
-    <row r="15" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16">
         <v>14</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>86</v>
       </c>
       <c r="D15" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="E15" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="F15" s="17" t="s">
         <v>212</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>213</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
       <c r="I15" s="41" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
@@ -2468,7 +2471,7 @@
       <c r="N15" s="33"/>
       <c r="O15" s="33"/>
     </row>
-    <row r="16" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16">
         <v>15</v>
       </c>
@@ -2481,12 +2484,12 @@
       <c r="D16" s="20"/>
       <c r="E16" s="35"/>
       <c r="F16" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G16" s="76"/>
       <c r="H16" s="76"/>
       <c r="I16" s="42" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
@@ -2495,30 +2498,30 @@
       <c r="N16" s="33"/>
       <c r="O16" s="33"/>
     </row>
-    <row r="17" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16">
         <v>16</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>91</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E17" s="35"/>
       <c r="F17" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
       <c r="I17" s="34" t="s">
+        <v>218</v>
+      </c>
+      <c r="J17" s="30" t="s">
         <v>219</v>
-      </c>
-      <c r="J17" s="30" t="s">
-        <v>220</v>
       </c>
       <c r="K17" s="31"/>
       <c r="L17" s="31"/>
@@ -2526,22 +2529,22 @@
       <c r="N17" s="33"/>
       <c r="O17" s="33"/>
     </row>
-    <row r="18" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16">
         <v>17</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>94</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E18" s="35"/>
       <c r="F18" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
@@ -2553,12 +2556,12 @@
       <c r="N18" s="33"/>
       <c r="O18" s="33"/>
     </row>
-    <row r="19" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16">
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>74</v>
@@ -2566,15 +2569,15 @@
       <c r="D19" s="20"/>
       <c r="E19" s="35"/>
       <c r="F19" s="65" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
       <c r="I19" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="J19" s="30" t="s">
         <v>224</v>
-      </c>
-      <c r="J19" s="30" t="s">
-        <v>225</v>
       </c>
       <c r="K19" s="31"/>
       <c r="L19" s="31"/>
@@ -2582,7 +2585,7 @@
       <c r="N19" s="33"/>
       <c r="O19" s="33"/>
     </row>
-    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16">
         <v>19</v>
       </c>
@@ -2593,11 +2596,11 @@
         <v>98</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E20" s="35"/>
       <c r="F20" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
@@ -2609,12 +2612,12 @@
       <c r="N20" s="33"/>
       <c r="O20" s="33"/>
     </row>
-    <row r="21" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16">
         <v>20</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>101</v>
@@ -2622,7 +2625,7 @@
       <c r="D21" s="20"/>
       <c r="E21" s="35"/>
       <c r="F21" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
@@ -2634,7 +2637,7 @@
       <c r="N21" s="33"/>
       <c r="O21" s="33"/>
     </row>
-    <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16">
         <v>21</v>
       </c>
@@ -2655,27 +2658,27 @@
       <c r="N22" s="33"/>
       <c r="O22" s="33"/>
     </row>
-    <row r="23" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="16">
         <v>22</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>104</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E23" s="35"/>
       <c r="F23" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17"/>
       <c r="I23" s="34" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J23" s="30"/>
       <c r="K23" s="31"/>
@@ -2684,12 +2687,12 @@
       <c r="N23" s="33"/>
       <c r="O23" s="33"/>
     </row>
-    <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16">
         <v>23</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>106</v>
@@ -2697,12 +2700,12 @@
       <c r="D24" s="43"/>
       <c r="E24" s="35"/>
       <c r="F24" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="17"/>
       <c r="I24" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J24" s="40"/>
       <c r="K24" s="31"/>
@@ -2711,27 +2714,27 @@
       <c r="N24" s="33"/>
       <c r="O24" s="33"/>
     </row>
-    <row r="25" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16">
         <v>24</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>108</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="F25" s="17" t="s">
         <v>234</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>235</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="17"/>
       <c r="I25" s="36" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J25" s="30"/>
       <c r="K25" s="31"/>
@@ -2740,7 +2743,7 @@
       <c r="N25" s="33"/>
       <c r="O25" s="33"/>
     </row>
-    <row r="26" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16">
         <v>25</v>
       </c>
@@ -2751,11 +2754,11 @@
         <v>110</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E26" s="35"/>
       <c r="F26" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G26" s="17"/>
       <c r="H26" s="17"/>
@@ -2767,7 +2770,7 @@
       <c r="N26" s="33"/>
       <c r="O26" s="33"/>
     </row>
-    <row r="27" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16">
         <v>26</v>
       </c>
@@ -2788,7 +2791,7 @@
       <c r="N27" s="33"/>
       <c r="O27" s="33"/>
     </row>
-    <row r="28" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16">
         <v>27</v>
       </c>
@@ -2809,7 +2812,7 @@
       <c r="N28" s="33"/>
       <c r="O28" s="33"/>
     </row>
-    <row r="29" spans="1:15" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="16">
         <v>28</v>
       </c>
@@ -2820,16 +2823,16 @@
         <v>114</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E29" s="35"/>
       <c r="F29" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
       <c r="I29" s="36" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J29" s="30"/>
       <c r="K29" s="31"/>
@@ -2838,7 +2841,7 @@
       <c r="N29" s="33"/>
       <c r="O29" s="33"/>
     </row>
-    <row r="30" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16">
         <v>29</v>
       </c>
@@ -2851,7 +2854,7 @@
       <c r="D30" s="20"/>
       <c r="E30" s="35"/>
       <c r="F30" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="17"/>
@@ -2863,7 +2866,7 @@
       <c r="N30" s="33"/>
       <c r="O30" s="33"/>
     </row>
-    <row r="31" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16">
         <v>30</v>
       </c>
@@ -2876,12 +2879,12 @@
       <c r="D31" s="20"/>
       <c r="E31" s="35"/>
       <c r="F31" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G31" s="17"/>
       <c r="H31" s="17"/>
       <c r="I31" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J31" s="30"/>
       <c r="K31" s="31"/>
@@ -2890,7 +2893,7 @@
       <c r="N31" s="33"/>
       <c r="O31" s="33"/>
     </row>
-    <row r="32" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="16">
         <v>31</v>
       </c>
@@ -2911,7 +2914,7 @@
       <c r="N32" s="33"/>
       <c r="O32" s="33"/>
     </row>
-    <row r="33" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16">
         <v>32</v>
       </c>
@@ -2922,11 +2925,11 @@
         <v>121</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E33" s="35"/>
       <c r="F33" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G33" s="17"/>
       <c r="H33" s="17"/>
@@ -2938,7 +2941,7 @@
       <c r="N33" s="33"/>
       <c r="O33" s="33"/>
     </row>
-    <row r="34" spans="1:15" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16">
         <v>33</v>
       </c>
@@ -2949,16 +2952,16 @@
         <v>124</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E34" s="35"/>
       <c r="F34" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G34" s="17"/>
       <c r="H34" s="17"/>
       <c r="I34" s="36" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J34" s="40"/>
       <c r="K34" s="31"/>
@@ -2967,7 +2970,7 @@
       <c r="N34" s="33"/>
       <c r="O34" s="33"/>
     </row>
-    <row r="35" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="16">
         <v>34</v>
       </c>
@@ -2980,15 +2983,15 @@
       <c r="D35" s="20"/>
       <c r="E35" s="35"/>
       <c r="F35" s="17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G35" s="76"/>
       <c r="H35" s="76"/>
       <c r="I35" s="42" t="s">
+        <v>250</v>
+      </c>
+      <c r="J35" s="40" t="s">
         <v>251</v>
-      </c>
-      <c r="J35" s="40" t="s">
-        <v>252</v>
       </c>
       <c r="K35" s="31"/>
       <c r="L35" s="31"/>
@@ -2996,12 +2999,12 @@
       <c r="N35" s="33"/>
       <c r="O35" s="33"/>
     </row>
-    <row r="36" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16">
         <v>35</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>128</v>
@@ -3009,15 +3012,15 @@
       <c r="D36" s="17"/>
       <c r="E36" s="35"/>
       <c r="F36" s="17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G36" s="17"/>
       <c r="H36" s="17"/>
       <c r="I36" s="34" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J36" s="30" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="K36" s="31"/>
       <c r="L36" s="31"/>
@@ -3025,20 +3028,20 @@
       <c r="N36" s="33"/>
       <c r="O36" s="33"/>
     </row>
-    <row r="37" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16">
         <v>36</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>323</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>130</v>
+        <v>319</v>
+      </c>
+      <c r="C37" s="65" t="s">
+        <v>337</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="35"/>
-      <c r="F37" s="17" t="s">
-        <v>255</v>
+      <c r="F37" s="65" t="s">
+        <v>336</v>
       </c>
       <c r="G37" s="17"/>
       <c r="H37" s="17"/>
@@ -3050,7 +3053,7 @@
       <c r="N37" s="33"/>
       <c r="O37" s="33"/>
     </row>
-    <row r="38" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16">
         <v>37</v>
       </c>
@@ -3061,16 +3064,16 @@
         <v>133</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E38" s="35"/>
       <c r="F38" s="17" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G38" s="17"/>
       <c r="H38" s="17"/>
       <c r="I38" s="34" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J38" s="30"/>
       <c r="K38" s="31"/>
@@ -3079,7 +3082,7 @@
       <c r="N38" s="33"/>
       <c r="O38" s="33"/>
     </row>
-    <row r="39" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16">
         <v>38</v>
       </c>
@@ -3092,7 +3095,7 @@
       <c r="D39" s="20"/>
       <c r="E39" s="35"/>
       <c r="F39" s="17" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G39" s="17"/>
       <c r="H39" s="17"/>
@@ -3104,7 +3107,7 @@
       <c r="N39" s="33"/>
       <c r="O39" s="33"/>
     </row>
-    <row r="40" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16">
         <v>39</v>
       </c>
@@ -3125,7 +3128,7 @@
       <c r="N40" s="33"/>
       <c r="O40" s="33"/>
     </row>
-    <row r="41" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16">
         <v>40</v>
       </c>
@@ -3136,16 +3139,16 @@
         <v>138</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E41" s="67"/>
       <c r="F41" s="66" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G41" s="66"/>
       <c r="H41" s="66"/>
       <c r="I41" s="68" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J41" s="30"/>
       <c r="K41" s="31"/>
@@ -3154,7 +3157,7 @@
       <c r="N41" s="33"/>
       <c r="O41" s="33"/>
     </row>
-    <row r="42" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16">
         <v>41</v>
       </c>
@@ -3175,7 +3178,7 @@
       <c r="N42" s="33"/>
       <c r="O42" s="33"/>
     </row>
-    <row r="43" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16">
         <v>42</v>
       </c>
@@ -3196,25 +3199,25 @@
       <c r="N43" s="33"/>
       <c r="O43" s="33"/>
     </row>
-    <row r="44" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16">
         <v>43</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C44" s="65" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="35"/>
       <c r="F44" s="17" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G44" s="17"/>
       <c r="H44" s="17"/>
       <c r="I44" s="34" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J44" s="30"/>
       <c r="K44" s="31"/>
@@ -3223,7 +3226,7 @@
       <c r="N44" s="33"/>
       <c r="O44" s="33"/>
     </row>
-    <row r="45" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="16">
         <v>44</v>
       </c>
@@ -3231,17 +3234,17 @@
         <v>143</v>
       </c>
       <c r="C45" s="65" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="35"/>
       <c r="F45" s="17" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G45" s="17"/>
       <c r="H45" s="17"/>
       <c r="I45" s="34" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J45" s="30"/>
       <c r="K45" s="31"/>
@@ -3250,7 +3253,7 @@
       <c r="N45" s="33"/>
       <c r="O45" s="33"/>
     </row>
-    <row r="46" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16">
         <v>45</v>
       </c>
@@ -3262,10 +3265,10 @@
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="35" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G46" s="17"/>
       <c r="H46" s="17"/>
@@ -3277,7 +3280,7 @@
       <c r="N46" s="33"/>
       <c r="O46" s="33"/>
     </row>
-    <row r="47" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16">
         <v>46</v>
       </c>
@@ -3290,15 +3293,15 @@
       <c r="D47" s="20"/>
       <c r="E47" s="35"/>
       <c r="F47" s="36" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="G47" s="36"/>
       <c r="H47" s="36"/>
       <c r="I47" s="34" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J47" s="40" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K47" s="31"/>
       <c r="L47" s="31"/>
@@ -3306,7 +3309,7 @@
       <c r="N47" s="33"/>
       <c r="O47" s="33"/>
     </row>
-    <row r="48" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="16">
         <v>47</v>
       </c>
@@ -3317,16 +3320,16 @@
         <v>151</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E48" s="35"/>
       <c r="F48" s="17" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G48" s="17"/>
       <c r="H48" s="17"/>
       <c r="I48" s="34" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="J48" s="30"/>
       <c r="K48" s="31"/>
@@ -3335,25 +3338,25 @@
       <c r="N48" s="33"/>
       <c r="O48" s="33"/>
     </row>
-    <row r="49" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="16">
         <v>48</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>332</v>
-      </c>
-      <c r="C49" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="C49" s="66" t="s">
         <v>153</v>
       </c>
       <c r="D49" s="64"/>
       <c r="E49" s="35"/>
-      <c r="F49" s="17" t="s">
-        <v>273</v>
+      <c r="F49" s="66" t="s">
+        <v>335</v>
       </c>
       <c r="G49" s="17"/>
       <c r="H49" s="17"/>
       <c r="I49" s="34" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="J49" s="30"/>
       <c r="K49" s="31"/>
@@ -3362,7 +3365,7 @@
       <c r="N49" s="46"/>
       <c r="O49" s="33"/>
     </row>
-    <row r="50" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16">
         <v>49</v>
       </c>
@@ -3373,13 +3376,13 @@
         <v>155</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E50" s="35" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G50" s="17"/>
       <c r="H50" s="17"/>
@@ -3391,7 +3394,7 @@
       <c r="N50" s="33"/>
       <c r="O50" s="33"/>
     </row>
-    <row r="51" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="16">
         <v>50</v>
       </c>
@@ -3399,17 +3402,17 @@
         <v>156</v>
       </c>
       <c r="C51" s="74" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="35"/>
       <c r="F51" s="17" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G51" s="17"/>
       <c r="H51" s="17"/>
       <c r="I51" s="47" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="J51" s="30"/>
       <c r="K51" s="31"/>
@@ -3418,7 +3421,7 @@
       <c r="N51" s="33"/>
       <c r="O51" s="33"/>
     </row>
-    <row r="52" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="16">
         <v>51</v>
       </c>
@@ -3431,25 +3434,25 @@
       <c r="D52" s="20"/>
       <c r="E52" s="35"/>
       <c r="F52" s="17" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G52" s="17"/>
       <c r="H52" s="17"/>
       <c r="I52" s="47" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="J52" s="48" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K52" s="49" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="L52" s="31"/>
       <c r="M52" s="31"/>
       <c r="N52" s="33"/>
       <c r="O52" s="33"/>
     </row>
-    <row r="53" spans="1:15" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16">
         <v>52</v>
       </c>
@@ -3462,12 +3465,12 @@
       <c r="D53" s="20"/>
       <c r="E53" s="35"/>
       <c r="F53" s="17" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G53" s="17"/>
       <c r="H53" s="17"/>
       <c r="I53" s="34" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J53" s="30"/>
       <c r="K53" s="31"/>
@@ -3476,19 +3479,19 @@
       <c r="N53" s="33"/>
       <c r="O53" s="33"/>
     </row>
-    <row r="54" spans="1:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16">
         <v>53</v>
       </c>
       <c r="B54" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="C54" s="17" t="s">
-        <v>286</v>
+      <c r="C54" s="65" t="s">
+        <v>334</v>
       </c>
       <c r="D54" s="17"/>
       <c r="E54" s="73" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="F54" s="17"/>
       <c r="G54" s="17"/>
@@ -3501,19 +3504,19 @@
       <c r="N54" s="33"/>
       <c r="O54" s="33"/>
     </row>
-    <row r="55" spans="1:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="51">
         <v>54</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C55" s="73" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D55" s="17"/>
       <c r="E55" s="73" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F55" s="17"/>
       <c r="G55" s="17"/>
@@ -3526,7 +3529,7 @@
       <c r="N55" s="33"/>
       <c r="O55" s="33"/>
     </row>
-    <row r="56" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="23">
         <v>55</v>
       </c>
@@ -3538,10 +3541,10 @@
       </c>
       <c r="D56" s="20"/>
       <c r="E56" s="35" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G56" s="17"/>
       <c r="H56" s="17"/>
@@ -3553,27 +3556,27 @@
       <c r="N56" s="33"/>
       <c r="O56" s="33"/>
     </row>
-    <row r="57" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="23">
         <v>56</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C57" s="17" t="s">
         <v>166</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E57" s="50"/>
       <c r="F57" s="17" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="G57" s="17"/>
       <c r="H57" s="17"/>
       <c r="I57" s="34" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="J57" s="52"/>
       <c r="K57" s="31"/>
@@ -3582,30 +3585,30 @@
       <c r="N57" s="11"/>
       <c r="O57" s="11"/>
     </row>
-    <row r="58" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="23">
         <v>57</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C58" s="17" t="s">
         <v>169</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E58" s="35" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F58" s="17" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="G58" s="17" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="H58" s="17" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="I58" s="34"/>
       <c r="J58" s="30"/>
@@ -3615,7 +3618,7 @@
       <c r="N58" s="11"/>
       <c r="O58" s="11"/>
     </row>
-    <row r="59" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="24"/>
       <c r="B59" s="15"/>
       <c r="C59" s="53" t="s">
@@ -3642,14 +3645,14 @@
       <c r="N59" s="11"/>
       <c r="O59" s="11"/>
     </row>
-    <row r="60" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="24"/>
       <c r="B60" s="33"/>
       <c r="C60" s="30"/>
       <c r="D60" s="56"/>
       <c r="E60" s="33"/>
       <c r="F60" s="57" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="G60" s="57"/>
       <c r="H60" s="57"/>
@@ -3661,14 +3664,14 @@
       <c r="N60" s="11"/>
       <c r="O60" s="11"/>
     </row>
-    <row r="61" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="24"/>
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
       <c r="F61" s="57" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="G61" s="57"/>
       <c r="H61" s="57"/>
@@ -3680,14 +3683,14 @@
       <c r="N61" s="11"/>
       <c r="O61" s="11"/>
     </row>
-    <row r="62" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="24"/>
       <c r="B62" s="58"/>
       <c r="C62" s="15"/>
       <c r="D62" s="15"/>
       <c r="E62" s="59"/>
       <c r="F62" s="60" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="G62" s="77"/>
       <c r="H62" s="77"/>
@@ -3699,16 +3702,16 @@
       <c r="N62" s="11"/>
       <c r="O62" s="11"/>
     </row>
-    <row r="63" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="24" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B63" s="58"/>
       <c r="C63" s="15"/>
       <c r="D63" s="15"/>
       <c r="E63" s="59"/>
       <c r="F63" s="60" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="G63" s="77"/>
       <c r="H63" s="77"/>
@@ -3720,14 +3723,14 @@
       <c r="N63" s="11"/>
       <c r="O63" s="11"/>
     </row>
-    <row r="64" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="24"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
       <c r="F64" s="57" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="G64" s="57"/>
       <c r="H64" s="57"/>
@@ -3741,6 +3744,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3753,16 +3757,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="20.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16">
         <v>1</v>
       </c>
@@ -3780,7 +3784,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16">
         <v>2</v>
       </c>
@@ -3798,7 +3802,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>3</v>
       </c>
@@ -3816,7 +3820,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
         <v>4</v>
       </c>
@@ -3834,7 +3838,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>5</v>
       </c>
@@ -3852,7 +3856,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>6</v>
       </c>
@@ -3864,7 +3868,7 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>7</v>
       </c>
@@ -3884,7 +3888,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>8</v>
       </c>
@@ -3902,7 +3906,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>9</v>
       </c>
@@ -3920,7 +3924,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16">
         <v>10</v>
       </c>
@@ -3936,7 +3940,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16">
         <v>11</v>
       </c>
@@ -3952,7 +3956,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16">
         <v>12</v>
       </c>
@@ -3968,7 +3972,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16">
         <v>13</v>
       </c>
@@ -3986,7 +3990,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
         <v>14</v>
       </c>
@@ -4002,7 +4006,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16">
         <v>15</v>
       </c>
@@ -4020,7 +4024,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16">
         <v>16</v>
       </c>
@@ -4038,7 +4042,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16">
         <v>17</v>
       </c>
@@ -4054,7 +4058,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16">
         <v>18</v>
       </c>
@@ -4072,7 +4076,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16">
         <v>19</v>
       </c>
@@ -4092,7 +4096,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16">
         <v>20</v>
       </c>
@@ -4112,7 +4116,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16">
         <v>21</v>
       </c>
@@ -4124,7 +4128,7 @@
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16">
         <v>22</v>
       </c>
@@ -4144,7 +4148,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="16">
         <v>23</v>
       </c>
@@ -4164,7 +4168,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16">
         <v>24</v>
       </c>
@@ -4182,7 +4186,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16">
         <v>25</v>
       </c>
@@ -4198,7 +4202,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16">
         <v>26</v>
       </c>
@@ -4210,7 +4214,7 @@
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
     </row>
-    <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16">
         <v>27</v>
       </c>
@@ -4222,7 +4226,7 @@
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16">
         <v>28</v>
       </c>
@@ -4238,7 +4242,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="16">
         <v>29</v>
       </c>
@@ -4254,7 +4258,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16">
         <v>30</v>
       </c>
@@ -4270,7 +4274,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16">
         <v>31</v>
       </c>
@@ -4282,7 +4286,7 @@
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="16">
         <v>32</v>
       </c>
@@ -4300,7 +4304,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16">
         <v>33</v>
       </c>
@@ -4318,7 +4322,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16">
         <v>34</v>
       </c>
@@ -4334,7 +4338,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="16">
         <v>35</v>
       </c>
@@ -4352,7 +4356,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16">
         <v>36</v>
       </c>
@@ -4370,7 +4374,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16">
         <v>37</v>
       </c>
@@ -4386,7 +4390,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16">
         <v>38</v>
       </c>
@@ -4402,7 +4406,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16">
         <v>39</v>
       </c>
@@ -4416,7 +4420,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
         <v>136</v>
       </c>
@@ -4432,7 +4436,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16">
         <v>41</v>
       </c>
@@ -4444,7 +4448,7 @@
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
     </row>
-    <row r="42" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16">
         <v>42</v>
       </c>
@@ -4456,7 +4460,7 @@
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
     </row>
-    <row r="43" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16">
         <v>43</v>
       </c>
@@ -4470,7 +4474,7 @@
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
     </row>
-    <row r="44" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16">
         <v>44</v>
       </c>
@@ -4488,7 +4492,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="16">
         <v>1</v>
       </c>
@@ -4504,7 +4508,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16">
         <v>46</v>
       </c>
@@ -4520,7 +4524,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16">
         <v>47</v>
       </c>
@@ -4536,7 +4540,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="16">
         <v>115</v>
       </c>
@@ -4552,7 +4556,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="16">
         <v>75</v>
       </c>
@@ -4568,7 +4572,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16">
         <v>50</v>
       </c>
@@ -4584,7 +4588,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="16">
         <v>81</v>
       </c>
@@ -4600,7 +4604,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="16">
         <v>74</v>
       </c>
@@ -4616,7 +4620,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16"/>
       <c r="B53" s="21" t="s">
         <v>162</v>
@@ -4626,7 +4630,7 @@
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
     </row>
-    <row r="54" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="23">
         <v>68</v>
       </c>
@@ -4642,7 +4646,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="23"/>
       <c r="B55" s="20" t="s">
         <v>165</v>
@@ -4658,7 +4662,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="23">
         <v>66</v>
       </c>
@@ -4674,7 +4678,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="24"/>
       <c r="B57" s="15"/>
       <c r="C57" s="15" t="s">
@@ -4698,14 +4702,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>44</v>
       </c>
@@ -4716,7 +4720,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>47</v>
       </c>
@@ -4727,7 +4731,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>50</v>
       </c>
@@ -4738,7 +4742,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>53</v>
       </c>
@@ -4749,102 +4753,102 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
     </row>
-    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
     </row>
-    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
     </row>
-    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
     </row>
-    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
     </row>
-    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
     </row>
-    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
     </row>
-    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
     </row>
-    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
     </row>
-    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -4863,16 +4867,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -4883,7 +4887,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -4900,7 +4904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
@@ -4917,7 +4921,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
@@ -4932,7 +4936,7 @@
       </c>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>14</v>
       </c>
@@ -4945,7 +4949,7 @@
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="11" t="s">
         <v>17</v>
@@ -4956,7 +4960,7 @@
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="11" t="s">
         <v>19</v>
@@ -4967,7 +4971,7 @@
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="11" t="s">
         <v>21</v>
@@ -4978,7 +4982,7 @@
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="11" t="s">
         <v>23</v>
@@ -4989,7 +4993,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11" t="s">
@@ -4998,7 +5002,7 @@
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11" t="s">
@@ -5007,7 +5011,7 @@
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11" t="s">
@@ -5016,7 +5020,7 @@
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
     </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11" t="s">
@@ -5025,7 +5029,7 @@
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
     </row>
-    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11" t="s">
@@ -5034,7 +5038,7 @@
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
     </row>
-    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11" t="s">
@@ -5043,7 +5047,7 @@
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11" t="s">
@@ -5052,7 +5056,7 @@
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11" t="s">
@@ -5061,7 +5065,7 @@
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
     </row>
-    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11" t="s">
@@ -5070,7 +5074,7 @@
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11" t="s">
@@ -5079,7 +5083,7 @@
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11" t="s">
@@ -5088,7 +5092,7 @@
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11" t="s">
@@ -5097,7 +5101,7 @@
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11" t="s">
@@ -5106,7 +5110,7 @@
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11" t="s">
@@ -5115,7 +5119,7 @@
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11" t="s">
@@ -5124,7 +5128,7 @@
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11" t="s">
@@ -5133,7 +5137,7 @@
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11" t="s">
@@ -5142,7 +5146,7 @@
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11" t="s">
@@ -5151,7 +5155,7 @@
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11" t="s">
@@ -5160,7 +5164,7 @@
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11" t="s">
@@ -5169,7 +5173,7 @@
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11" t="s">
@@ -5178,7 +5182,7 @@
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11" t="s">

</xml_diff>

<commit_message>
upload solve whatsapp problem & changer alert type order
</commit_message>
<xml_diff>
--- a/lists/IP echipamente statii.xlsx
+++ b/lists/IP echipamente statii.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\TPL_Alerts2.0\lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9075D26C-6D4C-4326-B83F-090E94AF7386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A35BF5-4654-4B1A-869C-17B46ED794A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="341">
   <si>
     <t>Buffer maro</t>
   </si>
@@ -811,9 +811,6 @@
     <t>192.168.45.49 statie                192.168.45.63</t>
   </si>
   <si>
-    <t>192.168.25.38</t>
-  </si>
-  <si>
     <t>192.168.25.39 statie 192.168.25.58 cctv</t>
   </si>
   <si>
@@ -868,9 +865,6 @@
     <t>fibra de la scoala</t>
   </si>
   <si>
-    <t>192.168.45.39</t>
-  </si>
-  <si>
     <t>192.168.45.40  statie                   192.168.45.41 cctv</t>
   </si>
   <si>
@@ -1003,9 +997,6 @@
     <t>x192.168.25.37</t>
   </si>
   <si>
-    <t>x192.168.35.63</t>
-  </si>
-  <si>
     <t>x192.168.25.45</t>
   </si>
   <si>
@@ -1037,6 +1028,24 @@
   </si>
   <si>
     <t>x192.168.55.31</t>
+  </si>
+  <si>
+    <t>x192.168.35.28</t>
+  </si>
+  <si>
+    <t>x192.168.45.38</t>
+  </si>
+  <si>
+    <t>x192.168.45.39</t>
+  </si>
+  <si>
+    <t>x192.168.25.38</t>
+  </si>
+  <si>
+    <t>x192.168.45.25</t>
+  </si>
+  <si>
+    <t>x192.168.25.44</t>
   </si>
 </sst>
 </file>
@@ -1479,7 +1488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1693,9 +1702,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2013,28 +2019,28 @@
   </sheetPr>
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" style="63" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="19.44140625" style="63" customWidth="1"/>
-    <col min="9" max="9" width="21.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.90625" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.90625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="17.36328125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" style="63" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19.453125" style="63" customWidth="1"/>
+    <col min="9" max="9" width="21.08984375" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.90625" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.6328125" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.54296875" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="13.54296875" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>171</v>
       </c>
@@ -2053,11 +2059,11 @@
       <c r="F1" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="75" t="s">
-        <v>329</v>
-      </c>
-      <c r="H1" s="75" t="s">
-        <v>330</v>
+      <c r="G1" s="74" t="s">
+        <v>326</v>
+      </c>
+      <c r="H1" s="74" t="s">
+        <v>327</v>
       </c>
       <c r="I1" s="29" t="s">
         <v>47</v>
@@ -2071,7 +2077,7 @@
       <c r="N1" s="33"/>
       <c r="O1" s="33"/>
     </row>
-    <row r="2" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -2102,12 +2108,12 @@
       <c r="N2" s="33"/>
       <c r="O2" s="33"/>
     </row>
-    <row r="3" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16">
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>60</v>
@@ -2133,22 +2139,22 @@
       <c r="N3" s="33"/>
       <c r="O3" s="33"/>
     </row>
-    <row r="4" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="16">
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="66" t="s">
-        <v>62</v>
+      <c r="C4" s="65" t="s">
+        <v>335</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="66" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F4" s="65" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
@@ -2166,12 +2172,12 @@
       <c r="N4" s="33"/>
       <c r="O4" s="33"/>
     </row>
-    <row r="5" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="16">
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>64</v>
@@ -2199,12 +2205,12 @@
       <c r="N5" s="33"/>
       <c r="O5" s="33"/>
     </row>
-    <row r="6" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16">
         <v>5</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>66</v>
@@ -2226,7 +2232,7 @@
       <c r="N6" s="33"/>
       <c r="O6" s="33"/>
     </row>
-    <row r="7" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="16">
         <v>6</v>
       </c>
@@ -2247,12 +2253,12 @@
       <c r="N7" s="33"/>
       <c r="O7" s="33"/>
     </row>
-    <row r="8" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16">
         <v>7</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>69</v>
@@ -2272,12 +2278,12 @@
       <c r="N8" s="31"/>
       <c r="O8" s="33"/>
     </row>
-    <row r="9" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="16">
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>72</v>
@@ -2299,7 +2305,7 @@
       <c r="N9" s="31"/>
       <c r="O9" s="33"/>
     </row>
-    <row r="10" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="16">
         <v>9</v>
       </c>
@@ -2328,7 +2334,7 @@
       <c r="N10" s="31"/>
       <c r="O10" s="33"/>
     </row>
-    <row r="11" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="16">
         <v>10</v>
       </c>
@@ -2355,7 +2361,7 @@
       <c r="N11" s="31"/>
       <c r="O11" s="33"/>
     </row>
-    <row r="12" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="16">
         <v>11</v>
       </c>
@@ -2380,12 +2386,12 @@
       <c r="N12" s="31"/>
       <c r="O12" s="33"/>
     </row>
-    <row r="13" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16">
         <v>12</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>81</v>
@@ -2411,12 +2417,12 @@
       <c r="N13" s="31"/>
       <c r="O13" s="33"/>
     </row>
-    <row r="14" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="16">
         <v>13</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>83</v>
@@ -2440,12 +2446,12 @@
       <c r="N14" s="33"/>
       <c r="O14" s="33"/>
     </row>
-    <row r="15" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16">
         <v>14</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>86</v>
@@ -2471,7 +2477,7 @@
       <c r="N15" s="33"/>
       <c r="O15" s="33"/>
     </row>
-    <row r="16" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="16">
         <v>15</v>
       </c>
@@ -2486,8 +2492,8 @@
       <c r="F16" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="G16" s="76"/>
-      <c r="H16" s="76"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="75"/>
       <c r="I16" s="42" t="s">
         <v>215</v>
       </c>
@@ -2498,12 +2504,12 @@
       <c r="N16" s="33"/>
       <c r="O16" s="33"/>
     </row>
-    <row r="17" spans="1:15" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16">
         <v>16</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>91</v>
@@ -2529,12 +2535,12 @@
       <c r="N17" s="33"/>
       <c r="O17" s="33"/>
     </row>
-    <row r="18" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16">
         <v>17</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>94</v>
@@ -2556,20 +2562,20 @@
       <c r="N18" s="33"/>
       <c r="O18" s="33"/>
     </row>
-    <row r="19" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="16">
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>74</v>
+      <c r="C19" s="65" t="s">
+        <v>340</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="35"/>
       <c r="F19" s="65" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
@@ -2585,7 +2591,7 @@
       <c r="N19" s="33"/>
       <c r="O19" s="33"/>
     </row>
-    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="16">
         <v>19</v>
       </c>
@@ -2612,12 +2618,12 @@
       <c r="N20" s="33"/>
       <c r="O20" s="33"/>
     </row>
-    <row r="21" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="16">
         <v>20</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>101</v>
@@ -2637,7 +2643,7 @@
       <c r="N21" s="33"/>
       <c r="O21" s="33"/>
     </row>
-    <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="16">
         <v>21</v>
       </c>
@@ -2658,12 +2664,12 @@
       <c r="N22" s="33"/>
       <c r="O22" s="33"/>
     </row>
-    <row r="23" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="16">
         <v>22</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>104</v>
@@ -2687,12 +2693,12 @@
       <c r="N23" s="33"/>
       <c r="O23" s="33"/>
     </row>
-    <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="16">
         <v>23</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>106</v>
@@ -2714,12 +2720,12 @@
       <c r="N24" s="33"/>
       <c r="O24" s="33"/>
     </row>
-    <row r="25" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="16">
         <v>24</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>108</v>
@@ -2743,7 +2749,7 @@
       <c r="N25" s="33"/>
       <c r="O25" s="33"/>
     </row>
-    <row r="26" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="16">
         <v>25</v>
       </c>
@@ -2770,7 +2776,7 @@
       <c r="N26" s="33"/>
       <c r="O26" s="33"/>
     </row>
-    <row r="27" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="16">
         <v>26</v>
       </c>
@@ -2791,7 +2797,7 @@
       <c r="N27" s="33"/>
       <c r="O27" s="33"/>
     </row>
-    <row r="28" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="16">
         <v>27</v>
       </c>
@@ -2812,7 +2818,7 @@
       <c r="N28" s="33"/>
       <c r="O28" s="33"/>
     </row>
-    <row r="29" spans="1:15" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="16">
         <v>28</v>
       </c>
@@ -2841,7 +2847,7 @@
       <c r="N29" s="33"/>
       <c r="O29" s="33"/>
     </row>
-    <row r="30" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="16">
         <v>29</v>
       </c>
@@ -2866,7 +2872,7 @@
       <c r="N30" s="33"/>
       <c r="O30" s="33"/>
     </row>
-    <row r="31" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="16">
         <v>30</v>
       </c>
@@ -2893,7 +2899,7 @@
       <c r="N31" s="33"/>
       <c r="O31" s="33"/>
     </row>
-    <row r="32" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="16">
         <v>31</v>
       </c>
@@ -2914,7 +2920,7 @@
       <c r="N32" s="33"/>
       <c r="O32" s="33"/>
     </row>
-    <row r="33" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="16">
         <v>32</v>
       </c>
@@ -2941,7 +2947,7 @@
       <c r="N33" s="33"/>
       <c r="O33" s="33"/>
     </row>
-    <row r="34" spans="1:15" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="16">
         <v>33</v>
       </c>
@@ -2970,23 +2976,23 @@
       <c r="N34" s="33"/>
       <c r="O34" s="33"/>
     </row>
-    <row r="35" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="16">
         <v>34</v>
       </c>
       <c r="B35" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="C35" s="17" t="s">
-        <v>127</v>
+      <c r="C35" s="65" t="s">
+        <v>339</v>
       </c>
       <c r="D35" s="20"/>
       <c r="E35" s="35"/>
       <c r="F35" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="G35" s="76"/>
-      <c r="H35" s="76"/>
+      <c r="G35" s="75"/>
+      <c r="H35" s="75"/>
       <c r="I35" s="42" t="s">
         <v>250</v>
       </c>
@@ -2999,12 +3005,12 @@
       <c r="N35" s="33"/>
       <c r="O35" s="33"/>
     </row>
-    <row r="36" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="16">
         <v>35</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>128</v>
@@ -3020,7 +3026,7 @@
         <v>253</v>
       </c>
       <c r="J36" s="30" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="K36" s="31"/>
       <c r="L36" s="31"/>
@@ -3028,20 +3034,20 @@
       <c r="N36" s="33"/>
       <c r="O36" s="33"/>
     </row>
-    <row r="37" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="16">
         <v>36</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C37" s="65" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="35"/>
       <c r="F37" s="65" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G37" s="17"/>
       <c r="H37" s="17"/>
@@ -3053,7 +3059,7 @@
       <c r="N37" s="33"/>
       <c r="O37" s="33"/>
     </row>
-    <row r="38" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="16">
         <v>37</v>
       </c>
@@ -3082,7 +3088,7 @@
       <c r="N38" s="33"/>
       <c r="O38" s="33"/>
     </row>
-    <row r="39" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="16">
         <v>38</v>
       </c>
@@ -3107,7 +3113,7 @@
       <c r="N39" s="33"/>
       <c r="O39" s="33"/>
     </row>
-    <row r="40" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="16">
         <v>39</v>
       </c>
@@ -3128,7 +3134,7 @@
       <c r="N40" s="33"/>
       <c r="O40" s="33"/>
     </row>
-    <row r="41" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="16">
         <v>40</v>
       </c>
@@ -3139,7 +3145,7 @@
         <v>138</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E41" s="67"/>
       <c r="F41" s="66" t="s">
@@ -3157,7 +3163,7 @@
       <c r="N41" s="33"/>
       <c r="O41" s="33"/>
     </row>
-    <row r="42" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="16">
         <v>41</v>
       </c>
@@ -3178,7 +3184,7 @@
       <c r="N42" s="33"/>
       <c r="O42" s="33"/>
     </row>
-    <row r="43" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="16">
         <v>42</v>
       </c>
@@ -3199,15 +3205,15 @@
       <c r="N43" s="33"/>
       <c r="O43" s="33"/>
     </row>
-    <row r="44" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="16">
         <v>43</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C44" s="65" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="35"/>
@@ -3226,7 +3232,7 @@
       <c r="N44" s="33"/>
       <c r="O44" s="33"/>
     </row>
-    <row r="45" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="16">
         <v>44</v>
       </c>
@@ -3234,17 +3240,17 @@
         <v>143</v>
       </c>
       <c r="C45" s="65" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="35"/>
-      <c r="F45" s="17" t="s">
-        <v>262</v>
+      <c r="F45" s="65" t="s">
+        <v>338</v>
       </c>
       <c r="G45" s="17"/>
       <c r="H45" s="17"/>
       <c r="I45" s="34" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J45" s="30"/>
       <c r="K45" s="31"/>
@@ -3253,7 +3259,7 @@
       <c r="N45" s="33"/>
       <c r="O45" s="33"/>
     </row>
-    <row r="46" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="16">
         <v>45</v>
       </c>
@@ -3265,10 +3271,10 @@
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="F46" s="17" t="s">
         <v>264</v>
-      </c>
-      <c r="F46" s="17" t="s">
-        <v>265</v>
       </c>
       <c r="G46" s="17"/>
       <c r="H46" s="17"/>
@@ -3280,7 +3286,7 @@
       <c r="N46" s="33"/>
       <c r="O46" s="33"/>
     </row>
-    <row r="47" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="16">
         <v>46</v>
       </c>
@@ -3293,15 +3299,15 @@
       <c r="D47" s="20"/>
       <c r="E47" s="35"/>
       <c r="F47" s="36" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G47" s="36"/>
       <c r="H47" s="36"/>
       <c r="I47" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="J47" s="40" t="s">
         <v>266</v>
-      </c>
-      <c r="J47" s="40" t="s">
-        <v>267</v>
       </c>
       <c r="K47" s="31"/>
       <c r="L47" s="31"/>
@@ -3309,7 +3315,7 @@
       <c r="N47" s="33"/>
       <c r="O47" s="33"/>
     </row>
-    <row r="48" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="16">
         <v>47</v>
       </c>
@@ -3320,16 +3326,16 @@
         <v>151</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E48" s="35"/>
       <c r="F48" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G48" s="17"/>
       <c r="H48" s="17"/>
       <c r="I48" s="34" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J48" s="30"/>
       <c r="K48" s="31"/>
@@ -3338,12 +3344,12 @@
       <c r="N48" s="33"/>
       <c r="O48" s="33"/>
     </row>
-    <row r="49" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="16">
         <v>48</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C49" s="66" t="s">
         <v>153</v>
@@ -3351,12 +3357,12 @@
       <c r="D49" s="64"/>
       <c r="E49" s="35"/>
       <c r="F49" s="66" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G49" s="17"/>
       <c r="H49" s="17"/>
       <c r="I49" s="34" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J49" s="30"/>
       <c r="K49" s="31"/>
@@ -3365,7 +3371,7 @@
       <c r="N49" s="46"/>
       <c r="O49" s="33"/>
     </row>
-    <row r="50" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="16">
         <v>49</v>
       </c>
@@ -3376,13 +3382,13 @@
         <v>155</v>
       </c>
       <c r="D50" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="E50" s="35" t="s">
         <v>272</v>
       </c>
-      <c r="E50" s="35" t="s">
+      <c r="F50" s="17" t="s">
         <v>273</v>
-      </c>
-      <c r="F50" s="17" t="s">
-        <v>274</v>
       </c>
       <c r="G50" s="17"/>
       <c r="H50" s="17"/>
@@ -3394,25 +3400,25 @@
       <c r="N50" s="33"/>
       <c r="O50" s="33"/>
     </row>
-    <row r="51" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="16">
         <v>50</v>
       </c>
       <c r="B51" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="C51" s="74" t="s">
-        <v>326</v>
+      <c r="C51" s="66" t="s">
+        <v>157</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="35"/>
       <c r="F51" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G51" s="17"/>
       <c r="H51" s="17"/>
       <c r="I51" s="47" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J51" s="30"/>
       <c r="K51" s="31"/>
@@ -3421,7 +3427,7 @@
       <c r="N51" s="33"/>
       <c r="O51" s="33"/>
     </row>
-    <row r="52" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="16">
         <v>51</v>
       </c>
@@ -3434,43 +3440,43 @@
       <c r="D52" s="20"/>
       <c r="E52" s="35"/>
       <c r="F52" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G52" s="17"/>
       <c r="H52" s="17"/>
       <c r="I52" s="47" t="s">
+        <v>277</v>
+      </c>
+      <c r="J52" s="48" t="s">
         <v>278</v>
       </c>
-      <c r="J52" s="48" t="s">
+      <c r="K52" s="49" t="s">
         <v>279</v>
-      </c>
-      <c r="K52" s="49" t="s">
-        <v>280</v>
       </c>
       <c r="L52" s="31"/>
       <c r="M52" s="31"/>
       <c r="N52" s="33"/>
       <c r="O52" s="33"/>
     </row>
-    <row r="53" spans="1:15" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="16">
         <v>52</v>
       </c>
       <c r="B53" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="C53" s="17" t="s">
-        <v>161</v>
+      <c r="C53" s="65" t="s">
+        <v>336</v>
       </c>
       <c r="D53" s="20"/>
       <c r="E53" s="35"/>
-      <c r="F53" s="17" t="s">
-        <v>281</v>
+      <c r="F53" s="65" t="s">
+        <v>337</v>
       </c>
       <c r="G53" s="17"/>
       <c r="H53" s="17"/>
       <c r="I53" s="34" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J53" s="30"/>
       <c r="K53" s="31"/>
@@ -3479,7 +3485,7 @@
       <c r="N53" s="33"/>
       <c r="O53" s="33"/>
     </row>
-    <row r="54" spans="1:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="16">
         <v>53</v>
       </c>
@@ -3487,11 +3493,11 @@
         <v>162</v>
       </c>
       <c r="C54" s="65" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D54" s="17"/>
       <c r="E54" s="73" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F54" s="17"/>
       <c r="G54" s="17"/>
@@ -3504,19 +3510,19 @@
       <c r="N54" s="33"/>
       <c r="O54" s="33"/>
     </row>
-    <row r="55" spans="1:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="51">
         <v>54</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C55" s="73" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D55" s="17"/>
       <c r="E55" s="73" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F55" s="17"/>
       <c r="G55" s="17"/>
@@ -3529,7 +3535,7 @@
       <c r="N55" s="33"/>
       <c r="O55" s="33"/>
     </row>
-    <row r="56" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="23">
         <v>55</v>
       </c>
@@ -3541,10 +3547,10 @@
       </c>
       <c r="D56" s="20"/>
       <c r="E56" s="35" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G56" s="17"/>
       <c r="H56" s="17"/>
@@ -3556,27 +3562,27 @@
       <c r="N56" s="33"/>
       <c r="O56" s="33"/>
     </row>
-    <row r="57" spans="1:15" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" ht="40.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="23">
         <v>56</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C57" s="17" t="s">
         <v>166</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E57" s="50"/>
       <c r="F57" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G57" s="17"/>
       <c r="H57" s="17"/>
       <c r="I57" s="34" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J57" s="52"/>
       <c r="K57" s="31"/>
@@ -3585,30 +3591,30 @@
       <c r="N57" s="11"/>
       <c r="O57" s="11"/>
     </row>
-    <row r="58" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="23">
         <v>57</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C58" s="17" t="s">
         <v>169</v>
       </c>
       <c r="D58" s="20" t="s">
+        <v>290</v>
+      </c>
+      <c r="E58" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="F58" s="17" t="s">
         <v>292</v>
       </c>
-      <c r="E58" s="35" t="s">
-        <v>293</v>
-      </c>
-      <c r="F58" s="17" t="s">
-        <v>294</v>
-      </c>
       <c r="G58" s="17" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="H58" s="17" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="I58" s="34"/>
       <c r="J58" s="30"/>
@@ -3618,7 +3624,7 @@
       <c r="N58" s="11"/>
       <c r="O58" s="11"/>
     </row>
-    <row r="59" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="24"/>
       <c r="B59" s="15"/>
       <c r="C59" s="53" t="s">
@@ -3645,14 +3651,14 @@
       <c r="N59" s="11"/>
       <c r="O59" s="11"/>
     </row>
-    <row r="60" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="24"/>
       <c r="B60" s="33"/>
       <c r="C60" s="30"/>
       <c r="D60" s="56"/>
       <c r="E60" s="33"/>
       <c r="F60" s="57" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G60" s="57"/>
       <c r="H60" s="57"/>
@@ -3664,14 +3670,14 @@
       <c r="N60" s="11"/>
       <c r="O60" s="11"/>
     </row>
-    <row r="61" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="24"/>
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
       <c r="F61" s="57" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G61" s="57"/>
       <c r="H61" s="57"/>
@@ -3683,17 +3689,17 @@
       <c r="N61" s="11"/>
       <c r="O61" s="11"/>
     </row>
-    <row r="62" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="24"/>
       <c r="B62" s="58"/>
       <c r="C62" s="15"/>
       <c r="D62" s="15"/>
       <c r="E62" s="59"/>
       <c r="F62" s="60" t="s">
-        <v>297</v>
-      </c>
-      <c r="G62" s="77"/>
-      <c r="H62" s="77"/>
+        <v>295</v>
+      </c>
+      <c r="G62" s="76"/>
+      <c r="H62" s="76"/>
       <c r="I62" s="61"/>
       <c r="J62" s="62"/>
       <c r="K62" s="11"/>
@@ -3702,19 +3708,19 @@
       <c r="N62" s="11"/>
       <c r="O62" s="11"/>
     </row>
-    <row r="63" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="24" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B63" s="58"/>
       <c r="C63" s="15"/>
       <c r="D63" s="15"/>
       <c r="E63" s="59"/>
       <c r="F63" s="60" t="s">
-        <v>299</v>
-      </c>
-      <c r="G63" s="77"/>
-      <c r="H63" s="77"/>
+        <v>297</v>
+      </c>
+      <c r="G63" s="76"/>
+      <c r="H63" s="76"/>
       <c r="I63" s="61"/>
       <c r="J63" s="62"/>
       <c r="K63" s="11"/>
@@ -3723,14 +3729,14 @@
       <c r="N63" s="11"/>
       <c r="O63" s="11"/>
     </row>
-    <row r="64" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="24"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
       <c r="F64" s="57" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G64" s="57"/>
       <c r="H64" s="57"/>
@@ -3757,16 +3763,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="20.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.90625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.54296875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16">
         <v>1</v>
       </c>
@@ -3784,7 +3790,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="16">
         <v>2</v>
       </c>
@@ -3802,7 +3808,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16">
         <v>3</v>
       </c>
@@ -3820,7 +3826,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="16">
         <v>4</v>
       </c>
@@ -3838,7 +3844,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="16">
         <v>5</v>
       </c>
@@ -3856,7 +3862,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18">
         <v>6</v>
       </c>
@@ -3868,7 +3874,7 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="16">
         <v>7</v>
       </c>
@@ -3888,7 +3894,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16">
         <v>8</v>
       </c>
@@ -3906,7 +3912,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="16">
         <v>9</v>
       </c>
@@ -3924,7 +3930,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="16">
         <v>10</v>
       </c>
@@ -3940,7 +3946,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="16">
         <v>11</v>
       </c>
@@ -3956,7 +3962,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="16">
         <v>12</v>
       </c>
@@ -3972,7 +3978,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16">
         <v>13</v>
       </c>
@@ -3990,7 +3996,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="16">
         <v>14</v>
       </c>
@@ -4006,7 +4012,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16">
         <v>15</v>
       </c>
@@ -4024,7 +4030,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="16">
         <v>16</v>
       </c>
@@ -4042,7 +4048,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16">
         <v>17</v>
       </c>
@@ -4058,7 +4064,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16">
         <v>18</v>
       </c>
@@ -4076,7 +4082,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="16">
         <v>19</v>
       </c>
@@ -4096,7 +4102,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="16">
         <v>20</v>
       </c>
@@ -4116,7 +4122,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="16">
         <v>21</v>
       </c>
@@ -4128,7 +4134,7 @@
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="16">
         <v>22</v>
       </c>
@@ -4148,7 +4154,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="16">
         <v>23</v>
       </c>
@@ -4168,7 +4174,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="16">
         <v>24</v>
       </c>
@@ -4186,7 +4192,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="16">
         <v>25</v>
       </c>
@@ -4202,7 +4208,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="16">
         <v>26</v>
       </c>
@@ -4214,7 +4220,7 @@
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
     </row>
-    <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="16">
         <v>27</v>
       </c>
@@ -4226,7 +4232,7 @@
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="16">
         <v>28</v>
       </c>
@@ -4242,7 +4248,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="16">
         <v>29</v>
       </c>
@@ -4258,7 +4264,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="16">
         <v>30</v>
       </c>
@@ -4274,7 +4280,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="16">
         <v>31</v>
       </c>
@@ -4286,7 +4292,7 @@
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="16">
         <v>32</v>
       </c>
@@ -4304,7 +4310,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="16">
         <v>33</v>
       </c>
@@ -4322,7 +4328,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="16">
         <v>34</v>
       </c>
@@ -4338,7 +4344,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="16">
         <v>35</v>
       </c>
@@ -4356,7 +4362,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="16">
         <v>36</v>
       </c>
@@ -4374,7 +4380,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="16">
         <v>37</v>
       </c>
@@ -4390,7 +4396,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="16">
         <v>38</v>
       </c>
@@ -4406,7 +4412,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="16">
         <v>39</v>
       </c>
@@ -4420,7 +4426,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="16" t="s">
         <v>136</v>
       </c>
@@ -4436,7 +4442,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="16">
         <v>41</v>
       </c>
@@ -4448,7 +4454,7 @@
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
     </row>
-    <row r="42" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="16">
         <v>42</v>
       </c>
@@ -4460,7 +4466,7 @@
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
     </row>
-    <row r="43" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="16">
         <v>43</v>
       </c>
@@ -4474,7 +4480,7 @@
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
     </row>
-    <row r="44" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="16">
         <v>44</v>
       </c>
@@ -4492,7 +4498,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="16">
         <v>1</v>
       </c>
@@ -4508,7 +4514,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="16">
         <v>46</v>
       </c>
@@ -4524,7 +4530,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="16">
         <v>47</v>
       </c>
@@ -4540,7 +4546,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="16">
         <v>115</v>
       </c>
@@ -4556,7 +4562,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="16">
         <v>75</v>
       </c>
@@ -4572,7 +4578,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="16">
         <v>50</v>
       </c>
@@ -4588,7 +4594,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="16">
         <v>81</v>
       </c>
@@ -4604,7 +4610,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="16">
         <v>74</v>
       </c>
@@ -4620,7 +4626,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="16"/>
       <c r="B53" s="21" t="s">
         <v>162</v>
@@ -4630,7 +4636,7 @@
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
     </row>
-    <row r="54" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="23">
         <v>68</v>
       </c>
@@ -4646,7 +4652,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="23"/>
       <c r="B55" s="20" t="s">
         <v>165</v>
@@ -4662,7 +4668,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="23">
         <v>66</v>
       </c>
@@ -4678,7 +4684,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="24"/>
       <c r="B57" s="15"/>
       <c r="C57" s="15" t="s">
@@ -4702,14 +4708,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.90625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>44</v>
       </c>
@@ -4720,7 +4726,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>47</v>
       </c>
@@ -4731,7 +4737,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>50</v>
       </c>
@@ -4742,7 +4748,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>53</v>
       </c>
@@ -4753,102 +4759,102 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
     </row>
-    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
     </row>
-    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
     </row>
-    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
     </row>
-    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
     </row>
-    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
     </row>
-    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
     </row>
-    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="15"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
     </row>
-    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
     </row>
-    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="15"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="15"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="15"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="15"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="15"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="15"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="15"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -4867,16 +4873,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.90625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.54296875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.08984375" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.453125" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -4887,7 +4893,7 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -4904,7 +4910,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
@@ -4921,7 +4927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
@@ -4936,7 +4942,7 @@
       </c>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>14</v>
       </c>
@@ -4949,7 +4955,7 @@
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11"/>
       <c r="B6" s="11" t="s">
         <v>17</v>
@@ -4960,7 +4966,7 @@
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11"/>
       <c r="B7" s="11" t="s">
         <v>19</v>
@@ -4971,7 +4977,7 @@
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11"/>
       <c r="B8" s="11" t="s">
         <v>21</v>
@@ -4982,7 +4988,7 @@
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
       <c r="B9" s="11" t="s">
         <v>23</v>
@@ -4993,7 +4999,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11" t="s">
@@ -5002,7 +5008,7 @@
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11" t="s">
@@ -5011,7 +5017,7 @@
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11" t="s">
@@ -5020,7 +5026,7 @@
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
     </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11" t="s">
@@ -5029,7 +5035,7 @@
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
     </row>
-    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11" t="s">
@@ -5038,7 +5044,7 @@
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
     </row>
-    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11" t="s">
@@ -5047,7 +5053,7 @@
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11" t="s">
@@ -5056,7 +5062,7 @@
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
     </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11" t="s">
@@ -5065,7 +5071,7 @@
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
     </row>
-    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11" t="s">
@@ -5074,7 +5080,7 @@
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
     </row>
-    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11" t="s">
@@ -5083,7 +5089,7 @@
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11" t="s">
@@ -5092,7 +5098,7 @@
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11" t="s">
@@ -5101,7 +5107,7 @@
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11" t="s">
@@ -5110,7 +5116,7 @@
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11" t="s">
@@ -5119,7 +5125,7 @@
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11" t="s">
@@ -5128,7 +5134,7 @@
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11" t="s">
@@ -5137,7 +5143,7 @@
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11" t="s">
@@ -5146,7 +5152,7 @@
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11" t="s">
@@ -5155,7 +5161,7 @@
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11" t="s">
@@ -5164,7 +5170,7 @@
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11" t="s">
@@ -5173,7 +5179,7 @@
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11" t="s">
@@ -5182,7 +5188,7 @@
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11" t="s">

</xml_diff>

<commit_message>
pdf_parser temp fix for catedrala
</commit_message>
<xml_diff>
--- a/lists/IP echipamente statii.xlsx
+++ b/lists/IP echipamente statii.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\TPL_Alerts2.0\lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9077CAFC-B9BC-4ADA-AACD-E754F4F314FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4BFF0D-BC5B-400A-8D0C-4A87615BFBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista principala" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="372">
   <si>
     <t>Buffer maro</t>
   </si>
@@ -865,9 +865,6 @@
     <t>192.168.45.40  statie                   192.168.45.41 cctv</t>
   </si>
   <si>
-    <t>192.168.95.152</t>
-  </si>
-  <si>
     <t>Aleea Dumbravii gostat</t>
   </si>
   <si>
@@ -892,15 +889,6 @@
     <t>192.168.15.29 statie 192.168.15.30 cctv</t>
   </si>
   <si>
-    <t>192.168.35.70</t>
-  </si>
-  <si>
-    <t>192.168.95.147</t>
-  </si>
-  <si>
-    <t>192.168.35.71</t>
-  </si>
-  <si>
     <t>A1   15.10</t>
   </si>
   <si>
@@ -991,27 +979,15 @@
     <t>Releu Panou</t>
   </si>
   <si>
-    <t>192.168.35.53</t>
-  </si>
-  <si>
-    <t>192.168.35.52</t>
-  </si>
-  <si>
     <t>192.168.45.45</t>
   </si>
   <si>
-    <t>x192.168.45.38</t>
-  </si>
-  <si>
     <t>x192.168.45.39</t>
   </si>
   <si>
     <t>192.168.25.38</t>
   </si>
   <si>
-    <t>192.168.95.160</t>
-  </si>
-  <si>
     <t>192.168.35.30</t>
   </si>
   <si>
@@ -1024,12 +1000,6 @@
     <t>192.168.95.150</t>
   </si>
   <si>
-    <t>x192.168.45.28</t>
-  </si>
-  <si>
-    <t>x192.168.45.27</t>
-  </si>
-  <si>
     <t>Sala Sporturilor spre BDJ</t>
   </si>
   <si>
@@ -1072,46 +1042,103 @@
     <t>192.168.35.92</t>
   </si>
   <si>
-    <t>x192.168.35.87</t>
-  </si>
-  <si>
-    <t>x192.168.35.89</t>
-  </si>
-  <si>
-    <t>x192.168.35.83</t>
-  </si>
-  <si>
-    <t>x192.168.25.62</t>
-  </si>
-  <si>
-    <t>x192.168.25.64</t>
-  </si>
-  <si>
-    <t>x192.168.35.85</t>
-  </si>
-  <si>
     <t>Piata Mare</t>
   </si>
   <si>
     <t>x192.168.45.67</t>
   </si>
   <si>
-    <t>x192.168.45.68</t>
-  </si>
-  <si>
     <t>Pasarela Itcani</t>
   </si>
   <si>
     <t>x192.168.45.65</t>
   </si>
   <si>
-    <t>x192.168.45.69</t>
-  </si>
-  <si>
     <t>192.168.55.53</t>
   </si>
   <si>
-    <t>x192.168.35.90</t>
+    <t>192.168.25.62</t>
+  </si>
+  <si>
+    <t>192.168.25.64</t>
+  </si>
+  <si>
+    <t>192.168.35.87</t>
+  </si>
+  <si>
+    <t>192.168.35.89</t>
+  </si>
+  <si>
+    <t>192.168.35.83</t>
+  </si>
+  <si>
+    <t>192.168.35.85</t>
+  </si>
+  <si>
+    <t>192.168.35.90</t>
+  </si>
+  <si>
+    <t>192.168.45.28</t>
+  </si>
+  <si>
+    <t>192.168.45.69</t>
+  </si>
+  <si>
+    <t>192.168.45.68</t>
+  </si>
+  <si>
+    <t>Sc. Gen. Nr. 6 (Burdujeni)</t>
+  </si>
+  <si>
+    <t>x192.168.35.69</t>
+  </si>
+  <si>
+    <t>x192.168.35.70</t>
+  </si>
+  <si>
+    <t>x192.168.95.147</t>
+  </si>
+  <si>
+    <t>x192.168.35.71</t>
+  </si>
+  <si>
+    <t>x192.168.35.53</t>
+  </si>
+  <si>
+    <t>x192.168.35.52</t>
+  </si>
+  <si>
+    <t>x192.168.95.160</t>
+  </si>
+  <si>
+    <t>x192.168.95.152</t>
+  </si>
+  <si>
+    <t>192.168.35.84</t>
+  </si>
+  <si>
+    <t>192.168.45.66</t>
+  </si>
+  <si>
+    <t>192.168.45.64</t>
+  </si>
+  <si>
+    <t>192.168.35.86</t>
+  </si>
+  <si>
+    <t>192.168.35.88</t>
+  </si>
+  <si>
+    <t>192.168.35.82</t>
+  </si>
+  <si>
+    <t>192.168.25.63</t>
+  </si>
+  <si>
+    <t>192.168.25.61</t>
+  </si>
+  <si>
+    <t>x192.168.35.57</t>
   </si>
 </sst>
 </file>
@@ -1567,7 +1594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1674,12 +1701,6 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1689,9 +1710,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1796,6 +1814,42 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2104,23 +2158,23 @@
   </sheetPr>
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.90625" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.90625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="17.36328125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.90625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.453125" style="63" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="19.453125" style="63" customWidth="1"/>
-    <col min="9" max="9" width="21.08984375" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.81640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.81640625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="17" style="12" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" style="60" customWidth="1"/>
+    <col min="7" max="8" width="19.453125" style="60" customWidth="1"/>
+    <col min="9" max="9" width="21.1796875" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="44.453125" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.90625" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.6328125" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.54296875" style="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.54296875" style="12" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="13.54296875" style="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -2144,11 +2198,11 @@
       <c r="F1" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="73" t="s">
-        <v>320</v>
-      </c>
-      <c r="H1" s="73" t="s">
-        <v>321</v>
+      <c r="G1" s="70" t="s">
+        <v>316</v>
+      </c>
+      <c r="H1" s="70" t="s">
+        <v>317</v>
       </c>
       <c r="I1" s="29" t="s">
         <v>47</v>
@@ -2166,7 +2220,7 @@
       <c r="A2" s="16">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="76" t="s">
         <v>55</v>
       </c>
       <c r="C2" s="17" t="s">
@@ -2197,8 +2251,8 @@
       <c r="A3" s="16">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>337</v>
+      <c r="B3" s="76" t="s">
+        <v>327</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>60</v>
@@ -2228,18 +2282,18 @@
       <c r="A4" s="16">
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="62" t="s">
         <v>62</v>
       </c>
       <c r="D4" s="20"/>
-      <c r="E4" s="65" t="s">
-        <v>332</v>
-      </c>
-      <c r="F4" s="65" t="s">
-        <v>329</v>
+      <c r="E4" s="62" t="s">
+        <v>324</v>
+      </c>
+      <c r="F4" s="62" t="s">
+        <v>321</v>
       </c>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
@@ -2261,8 +2315,8 @@
       <c r="A5" s="16">
         <v>4</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>300</v>
+      <c r="B5" s="76" t="s">
+        <v>296</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>64</v>
@@ -2294,8 +2348,8 @@
       <c r="A6" s="16">
         <v>5</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>313</v>
+      <c r="B6" s="76" t="s">
+        <v>309</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>66</v>
@@ -2321,18 +2375,20 @@
       <c r="A7" s="16">
         <v>6</v>
       </c>
-      <c r="B7" s="68" t="s">
-        <v>336</v>
-      </c>
-      <c r="C7" s="64" t="s">
-        <v>352</v>
-      </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="71"/>
+      <c r="B7" s="81" t="s">
+        <v>326</v>
+      </c>
+      <c r="C7" s="62" t="s">
+        <v>344</v>
+      </c>
+      <c r="D7" s="83"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="62" t="s">
+        <v>370</v>
+      </c>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="64"/>
       <c r="J7" s="30"/>
       <c r="K7" s="31"/>
       <c r="L7" s="31"/>
@@ -2344,14 +2400,14 @@
       <c r="A8" s="16">
         <v>7</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>310</v>
+      <c r="B8" s="76" t="s">
+        <v>306</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>69</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="E8" s="35"/>
       <c r="F8" s="17" t="s">
@@ -2371,14 +2427,14 @@
       <c r="A9" s="16">
         <v>8</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>309</v>
-      </c>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="76" t="s">
+        <v>305</v>
+      </c>
+      <c r="C9" s="62" t="s">
         <v>72</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="E9" s="35"/>
       <c r="F9" s="17" t="s">
@@ -2400,7 +2456,7 @@
       <c r="A10" s="16">
         <v>9</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="76" t="s">
         <v>196</v>
       </c>
       <c r="C10" s="17" t="s">
@@ -2429,7 +2485,7 @@
       <c r="A11" s="16">
         <v>10</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="76" t="s">
         <v>76</v>
       </c>
       <c r="C11" s="17" t="s">
@@ -2456,14 +2512,14 @@
       <c r="A12" s="16">
         <v>11</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="76" t="s">
         <v>78</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>79</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>361</v>
+        <v>343</v>
       </c>
       <c r="E12" s="35"/>
       <c r="F12" s="17" t="s">
@@ -2483,14 +2539,14 @@
       <c r="A13" s="16">
         <v>12</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>304</v>
+      <c r="B13" s="76" t="s">
+        <v>300</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>81</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>203</v>
@@ -2504,7 +2560,7 @@
         <v>205</v>
       </c>
       <c r="J13" s="11"/>
-      <c r="K13" s="40" t="s">
+      <c r="K13" s="38" t="s">
         <v>206</v>
       </c>
       <c r="L13" s="31"/>
@@ -2516,8 +2572,8 @@
       <c r="A14" s="16">
         <v>13</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>311</v>
+      <c r="B14" s="76" t="s">
+        <v>307</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>83</v>
@@ -2545,8 +2601,8 @@
       <c r="A15" s="16">
         <v>14</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>306</v>
+      <c r="B15" s="76" t="s">
+        <v>302</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>86</v>
@@ -2562,7 +2618,7 @@
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
-      <c r="I15" s="41" t="s">
+      <c r="I15" s="39" t="s">
         <v>213</v>
       </c>
       <c r="J15" s="11"/>
@@ -2576,7 +2632,7 @@
       <c r="A16" s="16">
         <v>15</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="76" t="s">
         <v>87</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -2587,9 +2643,9 @@
       <c r="F16" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="G16" s="74"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="42" t="s">
+      <c r="G16" s="71"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="40" t="s">
         <v>215</v>
       </c>
       <c r="J16" s="11"/>
@@ -2599,12 +2655,12 @@
       <c r="N16" s="33"/>
       <c r="O16" s="33"/>
     </row>
-    <row r="17" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16">
         <v>16</v>
       </c>
-      <c r="B17" s="17" t="s">
-        <v>315</v>
+      <c r="B17" s="76" t="s">
+        <v>311</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>91</v>
@@ -2634,8 +2690,8 @@
       <c r="A18" s="16">
         <v>17</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>307</v>
+      <c r="B18" s="76" t="s">
+        <v>303</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>94</v>
@@ -2661,16 +2717,16 @@
       <c r="A19" s="16">
         <v>18</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="76" t="s">
         <v>222</v>
       </c>
-      <c r="C19" s="65" t="s">
+      <c r="C19" s="62" t="s">
         <v>74</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="35"/>
-      <c r="F19" s="65" t="s">
-        <v>330</v>
+      <c r="F19" s="62" t="s">
+        <v>322</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
@@ -2690,7 +2746,7 @@
       <c r="A20" s="16">
         <v>19</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="76" t="s">
         <v>97</v>
       </c>
       <c r="C20" s="17" t="s">
@@ -2717,8 +2773,8 @@
       <c r="A21" s="16">
         <v>20</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>308</v>
+      <c r="B21" s="76" t="s">
+        <v>304</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>101</v>
@@ -2742,18 +2798,20 @@
       <c r="A22" s="16">
         <v>21</v>
       </c>
-      <c r="B22" s="19" t="s">
-        <v>335</v>
-      </c>
-      <c r="C22" s="64" t="s">
-        <v>353</v>
-      </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="39"/>
+      <c r="B22" s="81" t="s">
+        <v>325</v>
+      </c>
+      <c r="C22" s="62" t="s">
+        <v>345</v>
+      </c>
+      <c r="D22" s="83"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="62" t="s">
+        <v>369</v>
+      </c>
+      <c r="G22" s="62"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="64"/>
       <c r="J22" s="30"/>
       <c r="K22" s="31"/>
       <c r="L22" s="31"/>
@@ -2765,22 +2823,22 @@
       <c r="A23" s="16">
         <v>22</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>312</v>
-      </c>
-      <c r="C23" s="17" t="s">
+      <c r="B23" s="81" t="s">
+        <v>308</v>
+      </c>
+      <c r="C23" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="83" t="s">
         <v>228</v>
       </c>
-      <c r="E23" s="35"/>
-      <c r="F23" s="17" t="s">
+      <c r="E23" s="63"/>
+      <c r="F23" s="62" t="s">
         <v>229</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="34" t="s">
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="64" t="s">
         <v>230</v>
       </c>
       <c r="J23" s="30"/>
@@ -2794,23 +2852,23 @@
       <c r="A24" s="16">
         <v>23</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>301</v>
-      </c>
-      <c r="C24" s="17" t="s">
+      <c r="B24" s="81" t="s">
+        <v>297</v>
+      </c>
+      <c r="C24" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="D24" s="43"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="17" t="s">
+      <c r="D24" s="84"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="62" t="s">
         <v>231</v>
       </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="34" t="s">
+      <c r="G24" s="62"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="64" t="s">
         <v>232</v>
       </c>
-      <c r="J24" s="40"/>
+      <c r="J24" s="38"/>
       <c r="K24" s="31"/>
       <c r="L24" s="31"/>
       <c r="M24" s="31"/>
@@ -2821,24 +2879,24 @@
       <c r="A25" s="16">
         <v>24</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>305</v>
-      </c>
-      <c r="C25" s="17" t="s">
+      <c r="B25" s="81" t="s">
+        <v>301</v>
+      </c>
+      <c r="C25" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="D25" s="17" t="s">
-        <v>344</v>
-      </c>
-      <c r="E25" s="17" t="s">
+      <c r="D25" s="62" t="s">
+        <v>334</v>
+      </c>
+      <c r="E25" s="62" t="s">
         <v>233</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="62" t="s">
         <v>234</v>
       </c>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="36" t="s">
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="85" t="s">
         <v>235</v>
       </c>
       <c r="J25" s="30"/>
@@ -2852,22 +2910,22 @@
       <c r="A26" s="16">
         <v>25</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="83" t="s">
         <v>236</v>
       </c>
-      <c r="E26" s="35"/>
-      <c r="F26" s="17" t="s">
+      <c r="E26" s="63"/>
+      <c r="F26" s="62" t="s">
         <v>237</v>
       </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="34"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="64"/>
       <c r="J26" s="30"/>
       <c r="K26" s="31"/>
       <c r="L26" s="31"/>
@@ -2879,18 +2937,20 @@
       <c r="A27" s="16">
         <v>26</v>
       </c>
-      <c r="B27" s="68" t="s">
+      <c r="B27" s="81" t="s">
         <v>111</v>
       </c>
-      <c r="C27" s="64" t="s">
-        <v>349</v>
-      </c>
-      <c r="D27" s="69"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="71"/>
+      <c r="C27" s="62" t="s">
+        <v>346</v>
+      </c>
+      <c r="D27" s="83"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="62" t="s">
+        <v>366</v>
+      </c>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="64"/>
       <c r="J27" s="30"/>
       <c r="K27" s="31"/>
       <c r="L27" s="31"/>
@@ -2902,18 +2962,20 @@
       <c r="A28" s="16">
         <v>27</v>
       </c>
-      <c r="B28" s="68" t="s">
+      <c r="B28" s="81" t="s">
         <v>112</v>
       </c>
-      <c r="C28" s="64" t="s">
-        <v>350</v>
-      </c>
-      <c r="D28" s="69"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="68"/>
-      <c r="I28" s="71"/>
+      <c r="C28" s="62" t="s">
+        <v>347</v>
+      </c>
+      <c r="D28" s="83"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="62" t="s">
+        <v>367</v>
+      </c>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="64"/>
       <c r="J28" s="30"/>
       <c r="K28" s="31"/>
       <c r="L28" s="31"/>
@@ -2921,26 +2983,26 @@
       <c r="N28" s="33"/>
       <c r="O28" s="33"/>
     </row>
-    <row r="29" spans="1:15" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="16">
         <v>28</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="62" t="s">
         <v>238</v>
       </c>
-      <c r="E29" s="35"/>
-      <c r="F29" s="17" t="s">
+      <c r="E29" s="63"/>
+      <c r="F29" s="62" t="s">
         <v>239</v>
       </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="36" t="s">
+      <c r="G29" s="62"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="85" t="s">
         <v>240</v>
       </c>
       <c r="J29" s="30"/>
@@ -2954,22 +3016,22 @@
       <c r="A30" s="16">
         <v>29</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="17" t="s">
-        <v>343</v>
-      </c>
-      <c r="E30" s="35"/>
-      <c r="F30" s="17" t="s">
+      <c r="D30" s="62" t="s">
+        <v>333</v>
+      </c>
+      <c r="E30" s="63"/>
+      <c r="F30" s="62" t="s">
         <v>241</v>
       </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="34"/>
+      <c r="G30" s="62"/>
+      <c r="H30" s="62"/>
+      <c r="I30" s="64"/>
       <c r="J30" s="30"/>
       <c r="K30" s="31"/>
       <c r="L30" s="31"/>
@@ -2981,22 +3043,22 @@
       <c r="A31" s="16">
         <v>30</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="82" t="s">
         <v>117</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="D31" s="17" t="s">
-        <v>342</v>
-      </c>
-      <c r="E31" s="35"/>
-      <c r="F31" s="17" t="s">
+      <c r="D31" s="62" t="s">
+        <v>332</v>
+      </c>
+      <c r="E31" s="63"/>
+      <c r="F31" s="62" t="s">
         <v>242</v>
       </c>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="34" t="s">
+      <c r="G31" s="62"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="64" t="s">
         <v>243</v>
       </c>
       <c r="J31" s="30"/>
@@ -3010,18 +3072,20 @@
       <c r="A32" s="16">
         <v>31</v>
       </c>
-      <c r="B32" s="69" t="s">
+      <c r="B32" s="82" t="s">
         <v>119</v>
       </c>
-      <c r="C32" s="64" t="s">
-        <v>351</v>
-      </c>
-      <c r="D32" s="69"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="71"/>
+      <c r="C32" s="62" t="s">
+        <v>348</v>
+      </c>
+      <c r="D32" s="83"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="62" t="s">
+        <v>368</v>
+      </c>
+      <c r="G32" s="62"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="64"/>
       <c r="J32" s="30"/>
       <c r="K32" s="31"/>
       <c r="L32" s="31"/>
@@ -3033,7 +3097,7 @@
       <c r="A33" s="16">
         <v>32</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="78" t="s">
         <v>120</v>
       </c>
       <c r="C33" s="17" t="s">
@@ -3056,12 +3120,12 @@
       <c r="N33" s="33"/>
       <c r="O33" s="33"/>
     </row>
-    <row r="34" spans="1:15" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="16">
         <v>33</v>
       </c>
-      <c r="B34" s="17" t="s">
-        <v>338</v>
+      <c r="B34" s="76" t="s">
+        <v>328</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>124</v>
@@ -3078,7 +3142,7 @@
       <c r="I34" s="36" t="s">
         <v>248</v>
       </c>
-      <c r="J34" s="40"/>
+      <c r="J34" s="38"/>
       <c r="K34" s="31"/>
       <c r="L34" s="31"/>
       <c r="M34" s="31"/>
@@ -3089,10 +3153,10 @@
       <c r="A35" s="16">
         <v>34</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="78" t="s">
         <v>126</v>
       </c>
-      <c r="C35" s="65" t="s">
+      <c r="C35" s="62" t="s">
         <v>127</v>
       </c>
       <c r="D35" s="20"/>
@@ -3100,12 +3164,12 @@
       <c r="F35" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="G35" s="74"/>
-      <c r="H35" s="74"/>
-      <c r="I35" s="42" t="s">
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="40" t="s">
         <v>250</v>
       </c>
-      <c r="J35" s="40" t="s">
+      <c r="J35" s="38" t="s">
         <v>251</v>
       </c>
       <c r="K35" s="31"/>
@@ -3118,8 +3182,8 @@
       <c r="A36" s="16">
         <v>35</v>
       </c>
-      <c r="B36" s="17" t="s">
-        <v>317</v>
+      <c r="B36" s="76" t="s">
+        <v>313</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>128</v>
@@ -3135,7 +3199,7 @@
         <v>253</v>
       </c>
       <c r="J36" s="30" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="K36" s="31"/>
       <c r="L36" s="31"/>
@@ -3147,16 +3211,16 @@
       <c r="A37" s="16">
         <v>36</v>
       </c>
-      <c r="B37" s="17" t="s">
-        <v>314</v>
-      </c>
-      <c r="C37" s="65" t="s">
+      <c r="B37" s="76" t="s">
+        <v>310</v>
+      </c>
+      <c r="C37" s="62" t="s">
         <v>130</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="35"/>
-      <c r="F37" s="65" t="s">
-        <v>331</v>
+      <c r="F37" s="62" t="s">
+        <v>323</v>
       </c>
       <c r="G37" s="17"/>
       <c r="H37" s="17"/>
@@ -3172,7 +3236,7 @@
       <c r="A38" s="16">
         <v>37</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="78" t="s">
         <v>132</v>
       </c>
       <c r="C38" s="17" t="s">
@@ -3201,16 +3265,16 @@
       <c r="A39" s="16">
         <v>38</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="78" t="s">
         <v>134</v>
       </c>
-      <c r="C39" s="64" t="s">
-        <v>334</v>
+      <c r="C39" s="62" t="s">
+        <v>135</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="35"/>
-      <c r="F39" s="64" t="s">
-        <v>333</v>
+      <c r="F39" s="62" t="s">
+        <v>351</v>
       </c>
       <c r="G39" s="17"/>
       <c r="H39" s="17"/>
@@ -3226,20 +3290,22 @@
       <c r="A40" s="16">
         <v>39</v>
       </c>
-      <c r="B40" s="19" t="s">
-        <v>339</v>
-      </c>
-      <c r="C40" s="64" t="s">
-        <v>354</v>
-      </c>
-      <c r="D40" s="64" t="s">
-        <v>362</v>
-      </c>
-      <c r="E40" s="38"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="39"/>
+      <c r="B40" s="81" t="s">
+        <v>329</v>
+      </c>
+      <c r="C40" s="62" t="s">
+        <v>349</v>
+      </c>
+      <c r="D40" s="62" t="s">
+        <v>350</v>
+      </c>
+      <c r="E40" s="63"/>
+      <c r="F40" s="62" t="s">
+        <v>363</v>
+      </c>
+      <c r="G40" s="62"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="64"/>
       <c r="J40" s="30"/>
       <c r="K40" s="31"/>
       <c r="L40" s="31"/>
@@ -3251,22 +3317,22 @@
       <c r="A41" s="16">
         <v>40</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="82" t="s">
         <v>137</v>
       </c>
-      <c r="C41" s="65" t="s">
+      <c r="C41" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="D41" s="17" t="s">
-        <v>303</v>
-      </c>
-      <c r="E41" s="66"/>
-      <c r="F41" s="65" t="s">
+      <c r="D41" s="62" t="s">
+        <v>299</v>
+      </c>
+      <c r="E41" s="63"/>
+      <c r="F41" s="62" t="s">
         <v>257</v>
       </c>
-      <c r="G41" s="65"/>
-      <c r="H41" s="65"/>
-      <c r="I41" s="67" t="s">
+      <c r="G41" s="62"/>
+      <c r="H41" s="62"/>
+      <c r="I41" s="64" t="s">
         <v>258</v>
       </c>
       <c r="J41" s="30"/>
@@ -3280,16 +3346,16 @@
       <c r="A42" s="16">
         <v>41</v>
       </c>
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="79" t="s">
         <v>139</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="39"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="67"/>
+      <c r="F42" s="65"/>
+      <c r="G42" s="65"/>
+      <c r="H42" s="65"/>
+      <c r="I42" s="68"/>
       <c r="J42" s="30"/>
       <c r="K42" s="31"/>
       <c r="L42" s="31"/>
@@ -3301,16 +3367,16 @@
       <c r="A43" s="16">
         <v>42</v>
       </c>
-      <c r="B43" s="21" t="s">
+      <c r="B43" s="79" t="s">
         <v>140</v>
       </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="39"/>
+      <c r="C43" s="65"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="65"/>
+      <c r="G43" s="65"/>
+      <c r="H43" s="65"/>
+      <c r="I43" s="68"/>
       <c r="J43" s="30"/>
       <c r="K43" s="31"/>
       <c r="L43" s="31"/>
@@ -3322,10 +3388,10 @@
       <c r="A44" s="16">
         <v>43</v>
       </c>
-      <c r="B44" s="17" t="s">
-        <v>302</v>
-      </c>
-      <c r="C44" s="65" t="s">
+      <c r="B44" s="76" t="s">
+        <v>298</v>
+      </c>
+      <c r="C44" s="62" t="s">
         <v>142</v>
       </c>
       <c r="D44" s="20"/>
@@ -3340,7 +3406,7 @@
       </c>
       <c r="J44" s="30"/>
       <c r="K44" s="31"/>
-      <c r="L44" s="44"/>
+      <c r="L44" s="41"/>
       <c r="M44" s="31"/>
       <c r="N44" s="33"/>
       <c r="O44" s="33"/>
@@ -3349,16 +3415,16 @@
       <c r="A45" s="16">
         <v>44</v>
       </c>
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="78" t="s">
         <v>143</v>
       </c>
-      <c r="C45" s="65" t="s">
+      <c r="C45" s="62" t="s">
         <v>144</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="35"/>
-      <c r="F45" s="65" t="s">
-        <v>327</v>
+      <c r="F45" s="62" t="s">
+        <v>320</v>
       </c>
       <c r="G45" s="17"/>
       <c r="H45" s="17"/>
@@ -3376,14 +3442,14 @@
       <c r="A46" s="16">
         <v>45</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="78" t="s">
         <v>146</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>147</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="E46" s="20" t="s">
         <v>262</v>
@@ -3405,23 +3471,23 @@
       <c r="A47" s="16">
         <v>46</v>
       </c>
-      <c r="B47" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>149</v>
+      <c r="B47" s="76" t="s">
+        <v>354</v>
+      </c>
+      <c r="C47" s="61" t="s">
+        <v>371</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="35"/>
       <c r="F47" s="36" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="G47" s="36"/>
       <c r="H47" s="36"/>
       <c r="I47" s="34" t="s">
         <v>264</v>
       </c>
-      <c r="J47" s="40" t="s">
+      <c r="J47" s="38" t="s">
         <v>265</v>
       </c>
       <c r="K47" s="31"/>
@@ -3434,7 +3500,7 @@
       <c r="A48" s="16">
         <v>47</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="78" t="s">
         <v>150</v>
       </c>
       <c r="C48" s="17" t="s">
@@ -3463,18 +3529,18 @@
       <c r="A49" s="16">
         <v>48</v>
       </c>
-      <c r="B49" s="17" t="s">
-        <v>319</v>
-      </c>
-      <c r="C49" s="65" t="s">
+      <c r="B49" s="76" t="s">
+        <v>315</v>
+      </c>
+      <c r="C49" s="62" t="s">
         <v>153</v>
       </c>
-      <c r="D49" s="65" t="s">
-        <v>346</v>
+      <c r="D49" s="62" t="s">
+        <v>336</v>
       </c>
       <c r="E49" s="35"/>
-      <c r="F49" s="65" t="s">
-        <v>324</v>
+      <c r="F49" s="62" t="s">
+        <v>318</v>
       </c>
       <c r="G49" s="17"/>
       <c r="H49" s="17"/>
@@ -3484,15 +3550,15 @@
       <c r="J49" s="30"/>
       <c r="K49" s="31"/>
       <c r="L49" s="31"/>
-      <c r="M49" s="45"/>
-      <c r="N49" s="46"/>
+      <c r="M49" s="42"/>
+      <c r="N49" s="43"/>
       <c r="O49" s="33"/>
     </row>
     <row r="50" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="16">
         <v>49</v>
       </c>
-      <c r="B50" s="20" t="s">
+      <c r="B50" s="78" t="s">
         <v>154</v>
       </c>
       <c r="C50" s="17" t="s">
@@ -3521,10 +3587,10 @@
       <c r="A51" s="16">
         <v>50</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="78" t="s">
         <v>156</v>
       </c>
-      <c r="C51" s="65" t="s">
+      <c r="C51" s="62" t="s">
         <v>157</v>
       </c>
       <c r="D51" s="20"/>
@@ -3534,7 +3600,7 @@
       </c>
       <c r="G51" s="17"/>
       <c r="H51" s="17"/>
-      <c r="I51" s="47" t="s">
+      <c r="I51" s="44" t="s">
         <v>274</v>
       </c>
       <c r="J51" s="30"/>
@@ -3548,7 +3614,7 @@
       <c r="A52" s="16">
         <v>51</v>
       </c>
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="78" t="s">
         <v>158</v>
       </c>
       <c r="C52" s="17" t="s">
@@ -3561,13 +3627,13 @@
       </c>
       <c r="G52" s="17"/>
       <c r="H52" s="17"/>
-      <c r="I52" s="47" t="s">
+      <c r="I52" s="44" t="s">
         <v>276</v>
       </c>
-      <c r="J52" s="48" t="s">
+      <c r="J52" s="45" t="s">
         <v>277</v>
       </c>
-      <c r="K52" s="49" t="s">
+      <c r="K52" s="46" t="s">
         <v>278</v>
       </c>
       <c r="L52" s="31"/>
@@ -3579,16 +3645,16 @@
       <c r="A53" s="16">
         <v>52</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="78" t="s">
         <v>160</v>
       </c>
-      <c r="C53" s="64" t="s">
-        <v>325</v>
+      <c r="C53" s="62" t="s">
+        <v>161</v>
       </c>
       <c r="D53" s="20"/>
       <c r="E53" s="35"/>
-      <c r="F53" s="64" t="s">
-        <v>326</v>
+      <c r="F53" s="61" t="s">
+        <v>319</v>
       </c>
       <c r="G53" s="17"/>
       <c r="H53" s="17"/>
@@ -3606,19 +3672,19 @@
       <c r="A54" s="16">
         <v>53</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="87" t="s">
         <v>162</v>
       </c>
-      <c r="C54" s="65" t="s">
-        <v>328</v>
-      </c>
-      <c r="D54" s="17"/>
-      <c r="E54" s="72" t="s">
-        <v>280</v>
-      </c>
-      <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
+      <c r="C54" s="61" t="s">
+        <v>361</v>
+      </c>
+      <c r="D54" s="61"/>
+      <c r="E54" s="80" t="s">
+        <v>362</v>
+      </c>
+      <c r="F54" s="61"/>
+      <c r="G54" s="61"/>
+      <c r="H54" s="61"/>
       <c r="I54" s="36"/>
       <c r="J54" s="30"/>
       <c r="K54" s="31"/>
@@ -3628,18 +3694,18 @@
       <c r="O54" s="33"/>
     </row>
     <row r="55" spans="1:15" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="51">
+      <c r="A55" s="48">
         <v>54</v>
       </c>
-      <c r="B55" s="20" t="s">
+      <c r="B55" s="78" t="s">
+        <v>280</v>
+      </c>
+      <c r="C55" s="69" t="s">
         <v>281</v>
       </c>
-      <c r="C55" s="72" t="s">
+      <c r="D55" s="17"/>
+      <c r="E55" s="69" t="s">
         <v>282</v>
-      </c>
-      <c r="D55" s="17"/>
-      <c r="E55" s="72" t="s">
-        <v>283</v>
       </c>
       <c r="F55" s="17"/>
       <c r="G55" s="17"/>
@@ -3656,20 +3722,20 @@
       <c r="A56" s="23">
         <v>55</v>
       </c>
-      <c r="B56" s="20" t="s">
+      <c r="B56" s="78" t="s">
         <v>163</v>
       </c>
       <c r="C56" s="17" t="s">
         <v>164</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="E56" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="F56" s="17" t="s">
         <v>284</v>
-      </c>
-      <c r="F56" s="17" t="s">
-        <v>285</v>
       </c>
       <c r="G56" s="17"/>
       <c r="H56" s="17"/>
@@ -3681,29 +3747,29 @@
       <c r="N56" s="33"/>
       <c r="O56" s="33"/>
     </row>
-    <row r="57" spans="1:15" ht="40.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" ht="40.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="23">
         <v>56</v>
       </c>
-      <c r="B57" s="17" t="s">
-        <v>298</v>
+      <c r="B57" s="76" t="s">
+        <v>294</v>
       </c>
       <c r="C57" s="17" t="s">
         <v>166</v>
       </c>
       <c r="D57" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="E57" s="47"/>
+      <c r="F57" s="17" t="s">
         <v>286</v>
-      </c>
-      <c r="E57" s="50"/>
-      <c r="F57" s="17" t="s">
-        <v>287</v>
       </c>
       <c r="G57" s="17"/>
       <c r="H57" s="17"/>
       <c r="I57" s="34" t="s">
-        <v>288</v>
-      </c>
-      <c r="J57" s="52"/>
+        <v>287</v>
+      </c>
+      <c r="J57" s="49"/>
       <c r="K57" s="31"/>
       <c r="L57" s="11"/>
       <c r="M57" s="11"/>
@@ -3714,26 +3780,26 @@
       <c r="A58" s="23">
         <v>57</v>
       </c>
-      <c r="B58" s="17" t="s">
-        <v>299</v>
-      </c>
-      <c r="C58" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="D58" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="E58" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="F58" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="G58" s="17" t="s">
-        <v>322</v>
-      </c>
-      <c r="H58" s="17" t="s">
-        <v>323</v>
+      <c r="B58" s="86" t="s">
+        <v>295</v>
+      </c>
+      <c r="C58" s="61" t="s">
+        <v>355</v>
+      </c>
+      <c r="D58" s="61" t="s">
+        <v>356</v>
+      </c>
+      <c r="E58" s="61" t="s">
+        <v>357</v>
+      </c>
+      <c r="F58" s="61" t="s">
+        <v>358</v>
+      </c>
+      <c r="G58" s="61" t="s">
+        <v>359</v>
+      </c>
+      <c r="H58" s="61" t="s">
+        <v>360</v>
       </c>
       <c r="I58" s="34"/>
       <c r="J58" s="30"/>
@@ -3747,58 +3813,64 @@
       <c r="A59" s="23">
         <v>58</v>
       </c>
-      <c r="B59" s="68" t="s">
-        <v>355</v>
-      </c>
-      <c r="C59" s="64" t="s">
-        <v>356</v>
-      </c>
-      <c r="D59" s="64" t="s">
-        <v>357</v>
-      </c>
-      <c r="E59" s="76"/>
-      <c r="F59" s="77"/>
-      <c r="G59" s="77"/>
-      <c r="H59" s="77"/>
-      <c r="I59" s="78"/>
+      <c r="B59" s="77" t="s">
+        <v>339</v>
+      </c>
+      <c r="C59" s="61" t="s">
+        <v>340</v>
+      </c>
+      <c r="D59" s="65" t="s">
+        <v>353</v>
+      </c>
+      <c r="E59" s="73"/>
+      <c r="F59" s="65" t="s">
+        <v>364</v>
+      </c>
+      <c r="G59" s="74"/>
+      <c r="H59" s="74"/>
+      <c r="I59" s="75"/>
       <c r="J59" s="30"/>
     </row>
     <row r="60" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="23"/>
-      <c r="B60" s="68" t="s">
-        <v>358</v>
-      </c>
-      <c r="C60" s="64" t="s">
-        <v>359</v>
-      </c>
-      <c r="D60" s="64" t="s">
-        <v>360</v>
-      </c>
-      <c r="E60" s="76"/>
-      <c r="F60" s="77"/>
-      <c r="G60" s="77"/>
-      <c r="H60" s="77"/>
-      <c r="I60" s="78"/>
+      <c r="A60" s="23">
+        <v>59</v>
+      </c>
+      <c r="B60" s="77" t="s">
+        <v>341</v>
+      </c>
+      <c r="C60" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="D60" s="65" t="s">
+        <v>352</v>
+      </c>
+      <c r="E60" s="73"/>
+      <c r="F60" s="65" t="s">
+        <v>365</v>
+      </c>
+      <c r="G60" s="74"/>
+      <c r="H60" s="74"/>
+      <c r="I60" s="75"/>
       <c r="J60" s="30"/>
     </row>
     <row r="61" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="24"/>
       <c r="B61" s="15"/>
-      <c r="C61" s="53" t="s">
+      <c r="C61" s="50" t="s">
         <v>170</v>
       </c>
-      <c r="D61" s="53" t="s">
+      <c r="D61" s="50" t="s">
         <v>173</v>
       </c>
-      <c r="E61" s="54" t="s">
+      <c r="E61" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="F61" s="55" t="s">
+      <c r="F61" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="G61" s="55"/>
-      <c r="H61" s="55"/>
-      <c r="I61" s="54" t="s">
+      <c r="G61" s="52"/>
+      <c r="H61" s="52"/>
+      <c r="I61" s="51" t="s">
         <v>47</v>
       </c>
       <c r="J61" s="15"/>
@@ -3812,13 +3884,13 @@
       <c r="A62" s="24"/>
       <c r="B62" s="33"/>
       <c r="C62" s="30"/>
-      <c r="D62" s="56"/>
+      <c r="D62" s="53"/>
       <c r="E62" s="33"/>
-      <c r="F62" s="57" t="s">
-        <v>292</v>
-      </c>
-      <c r="G62" s="57"/>
-      <c r="H62" s="57"/>
+      <c r="F62" s="54" t="s">
+        <v>288</v>
+      </c>
+      <c r="G62" s="54"/>
+      <c r="H62" s="54"/>
       <c r="I62" s="15"/>
       <c r="J62" s="15"/>
       <c r="K62" s="11"/>
@@ -3833,11 +3905,11 @@
       <c r="C63" s="15"/>
       <c r="D63" s="15"/>
       <c r="E63" s="15"/>
-      <c r="F63" s="57" t="s">
-        <v>293</v>
-      </c>
-      <c r="G63" s="57"/>
-      <c r="H63" s="57"/>
+      <c r="F63" s="54" t="s">
+        <v>289</v>
+      </c>
+      <c r="G63" s="54"/>
+      <c r="H63" s="54"/>
       <c r="I63" s="15"/>
       <c r="J63" s="15"/>
       <c r="K63" s="11"/>
@@ -3848,17 +3920,17 @@
     </row>
     <row r="64" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="24"/>
-      <c r="B64" s="58"/>
+      <c r="B64" s="55"/>
       <c r="C64" s="15"/>
       <c r="D64" s="15"/>
-      <c r="E64" s="59"/>
-      <c r="F64" s="60" t="s">
-        <v>294</v>
-      </c>
-      <c r="G64" s="75"/>
-      <c r="H64" s="75"/>
-      <c r="I64" s="61"/>
-      <c r="J64" s="62"/>
+      <c r="E64" s="56"/>
+      <c r="F64" s="57" t="s">
+        <v>290</v>
+      </c>
+      <c r="G64" s="72"/>
+      <c r="H64" s="72"/>
+      <c r="I64" s="58"/>
+      <c r="J64" s="59"/>
       <c r="K64" s="11"/>
       <c r="L64" s="11"/>
       <c r="M64" s="11"/>
@@ -3867,19 +3939,19 @@
     </row>
     <row r="65" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="B65" s="58"/>
+        <v>291</v>
+      </c>
+      <c r="B65" s="55"/>
       <c r="C65" s="15"/>
       <c r="D65" s="15"/>
-      <c r="E65" s="59"/>
-      <c r="F65" s="60" t="s">
-        <v>296</v>
-      </c>
-      <c r="G65" s="75"/>
-      <c r="H65" s="75"/>
-      <c r="I65" s="61"/>
-      <c r="J65" s="62"/>
+      <c r="E65" s="56"/>
+      <c r="F65" s="57" t="s">
+        <v>292</v>
+      </c>
+      <c r="G65" s="72"/>
+      <c r="H65" s="72"/>
+      <c r="I65" s="58"/>
+      <c r="J65" s="59"/>
       <c r="K65" s="11"/>
       <c r="L65" s="11"/>
       <c r="M65" s="11"/>
@@ -3892,11 +3964,11 @@
       <c r="C66" s="15"/>
       <c r="D66" s="15"/>
       <c r="E66" s="15"/>
-      <c r="F66" s="57" t="s">
-        <v>297</v>
-      </c>
-      <c r="G66" s="57"/>
-      <c r="H66" s="57"/>
+      <c r="F66" s="54" t="s">
+        <v>293</v>
+      </c>
+      <c r="G66" s="54"/>
+      <c r="H66" s="54"/>
       <c r="I66" s="15"/>
       <c r="J66" s="15"/>
       <c r="K66" s="11"/>
@@ -3924,7 +3996,7 @@
   <cols>
     <col min="1" max="1" width="13.54296875" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.90625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.81640625" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="20.54296875" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.54296875" style="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -4867,8 +4939,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.90625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.90625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5033,9 +5105,9 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="44.453125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.90625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.81640625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.54296875" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.08984375" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.1796875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.453125" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>